<commit_message>
Se crearon servicios para recorrido
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
   <si>
     <t>Recurso</t>
   </si>
@@ -446,6 +446,101 @@
   <si>
     <t>Agrega una parada a una ruta reemplazando la existente en esa posicion</t>
   </si>
+  <si>
+    <t>{
+ "Clave":"T3-1",
+    "Ruta":"T3",
+    "HoraDePartida":"23:58:00"
+}</t>
+  </si>
+  <si>
+    <t>{
+ "Clave":"T3-1",
+    "Parada":"ST17",
+    "HoraAnterior":"00:15:57",
+    "HoraNueva":"00:14:00"
+}</t>
+  </si>
+  <si>
+    <t>Crea un nuevo recorrido con horas preestablecidas según una velocidad promedio estimada. Devuelve true su la tarea se hizo correctamente</t>
+  </si>
+  <si>
+    <t>Edita la hora de una parada especificada y devuelve True si la tarea se hizo correctamente.</t>
+  </si>
+  <si>
+    <t>/post/recorridos/crear</t>
+  </si>
+  <si>
+    <t>/post/recorridos/editar</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/post/recorridos/crear</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/post/recorridos/editar</t>
+  </si>
+  <si>
+    <t>get/recorrido/consultar</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/get/recorridos/consultar</t>
+  </si>
+  <si>
+    <t>{
+  "Recorridos": [
+    {
+      "Clave": "HOLA",
+      "Ruta": "T3",
+      "HoraPartida": "23:54:59",
+      "Horario": {
+        "ST1": "23:54:59",
+        "ST2": "23:57:47",
+        "ST3": "00:02:52",
+        "ST4": "00:05:25",
+        "ST5": "00:10:11"
+      }
+    },
+    {
+      "Clave": "T3-1",
+      "Ruta": "T3",
+      "HoraPartida": "23:58:00",
+      "Horario": {
+        "ST1": "23:58:00",
+        "ST2": "00:00:48",
+        "ST17": "00:14:00",
+        "ST4": "00:23:29",
+        "ST5": "00:28:15"
+      }
+    }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>Obtiene todos los recorridos y sus horarios desde la base de datos.</t>
+  </si>
+  <si>
+    <t>get/recorrido/consultar/{$clave}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/get/recorridos/consultar/T3-1</t>
+  </si>
+  <si>
+    <t>{
+  "Clave": "T3-1",
+  "Ruta": "T3",
+  "HoraPartida": "23:58:00",
+  "Horario": {
+    "ST1": "23:58:00",
+    "ST2": "00:00:48",
+    "ST17": "00:14:00",
+    "ST4": "00:23:29",
+    "ST5": "00:28:15"
+  }
+}</t>
+  </si>
+  <si>
+    <t>Obtiene el recorrido especificado por el parametro de la url.</t>
+  </si>
 </sst>
 </file>
 
@@ -489,7 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -501,22 +596,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -848,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T69"/>
+  <dimension ref="A1:T97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45:S56"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +959,7 @@
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="18" max="18" width="32.7109375" customWidth="1"/>
-    <col min="19" max="19" width="32.140625" customWidth="1"/>
+    <col min="19" max="19" width="52.85546875" customWidth="1"/>
     <col min="20" max="20" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -869,15 +967,15 @@
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -891,26 +989,26 @@
       <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -920,28 +1018,28 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
       <c r="S3" s="2" t="s">
         <v>20</v>
       </c>
@@ -953,18 +1051,18 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="5" t="s">
         <v>13</v>
       </c>
@@ -980,26 +1078,26 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="C5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="5" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -1008,31 +1106,31 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="C6" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="5" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
@@ -1041,31 +1139,31 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="1" t="s">
+      <c r="S6" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -1080,25 +1178,25 @@
     </row>
     <row r="8" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="C8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -1113,25 +1211,25 @@
     </row>
     <row r="9" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="C9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
       <c r="K9" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -1146,25 +1244,25 @@
     </row>
     <row r="10" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -1179,25 +1277,25 @@
     </row>
     <row r="11" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="C11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
       <c r="K11" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1212,25 +1310,25 @@
     </row>
     <row r="12" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9" t="s">
+      <c r="C12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1245,25 +1343,25 @@
     </row>
     <row r="13" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9" t="s">
+      <c r="C13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1278,25 +1376,25 @@
     </row>
     <row r="14" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9" t="s">
+      <c r="C14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
       <c r="K14" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -1311,25 +1409,25 @@
     </row>
     <row r="15" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9" t="s">
+      <c r="C15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
       <c r="K15" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -1344,25 +1442,25 @@
     </row>
     <row r="16" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9" t="s">
+      <c r="C16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
       <c r="K16" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1377,25 +1475,25 @@
     </row>
     <row r="17" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9" t="s">
+      <c r="C17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
       <c r="K17" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -1408,20 +1506,28 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+    <row r="18" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -1429,117 +1535,131 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
-      <c r="S18" s="2"/>
-    </row>
-    <row r="19" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="S18" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="5" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S19" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>63</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="5"/>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
+      <c r="N21" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="T21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="5"/>
+      <c r="H22" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
+      <c r="N22" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="T22" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -1549,9 +1669,9 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -1571,9 +1691,9 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -1593,9 +1713,9 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
@@ -1615,9 +1735,9 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
@@ -1637,9 +1757,9 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
@@ -1659,9 +1779,9 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
@@ -1681,9 +1801,9 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
@@ -1703,9 +1823,9 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
@@ -1725,9 +1845,9 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
@@ -1740,52 +1860,38 @@
       <c r="T31" s="5"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
-      <c r="N32" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
-      <c r="T32" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="T32" s="5"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
@@ -1798,35 +1904,49 @@
       <c r="T33" s="5"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="5"/>
+      <c r="A34" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
+      <c r="K34" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
+      <c r="N34" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
+      <c r="T34" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -1844,11 +1964,11 @@
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -1866,11 +1986,11 @@
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
@@ -1888,11 +2008,11 @@
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
@@ -1910,11 +2030,11 @@
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -1932,11 +2052,11 @@
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -1954,11 +2074,11 @@
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
@@ -1976,11 +2096,11 @@
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
@@ -1998,11 +2118,11 @@
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
@@ -2020,11 +2140,11 @@
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
@@ -2040,49 +2160,35 @@
       <c r="T44" s="5"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="9" t="s">
-        <v>72</v>
-      </c>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
-      <c r="K45" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="K45" s="5"/>
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
-      <c r="N45" s="5" t="s">
-        <v>74</v>
-      </c>
+      <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
       <c r="S45" s="5"/>
-      <c r="T45" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="T45" s="5"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
@@ -2098,35 +2204,49 @@
       <c r="T46" s="5"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="5"/>
+      <c r="A47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
+      <c r="K47" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
+      <c r="N47" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="5"/>
       <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
+      <c r="T47" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
@@ -2144,11 +2264,11 @@
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
@@ -2166,11 +2286,11 @@
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
@@ -2188,11 +2308,11 @@
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
@@ -2210,11 +2330,11 @@
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
@@ -2232,11 +2352,11 @@
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
@@ -2254,11 +2374,11 @@
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
@@ -2276,11 +2396,11 @@
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
@@ -2298,11 +2418,11 @@
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
@@ -2318,49 +2438,35 @@
       <c r="T56" s="5"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
-      <c r="K57" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="K57" s="5"/>
       <c r="L57" s="5"/>
       <c r="M57" s="5"/>
-      <c r="N57" s="5" t="s">
-        <v>79</v>
-      </c>
+      <c r="N57" s="5"/>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
       <c r="Q57" s="5"/>
       <c r="R57" s="5"/>
       <c r="S57" s="5"/>
-      <c r="T57" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="T57" s="5"/>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
@@ -2376,35 +2482,49 @@
       <c r="T58" s="5"/>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="5"/>
+      <c r="A59" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
+      <c r="K59" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="L59" s="5"/>
       <c r="M59" s="5"/>
-      <c r="N59" s="5"/>
+      <c r="N59" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
       <c r="Q59" s="5"/>
       <c r="R59" s="5"/>
       <c r="S59" s="5"/>
-      <c r="T59" s="5"/>
+      <c r="T59" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
@@ -2422,11 +2542,11 @@
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
@@ -2444,11 +2564,11 @@
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
@@ -2466,11 +2586,11 @@
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
@@ -2488,11 +2608,11 @@
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
@@ -2510,11 +2630,11 @@
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
@@ -2532,11 +2652,11 @@
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
@@ -2554,11 +2674,11 @@
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
@@ -2576,11 +2696,11 @@
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
@@ -2598,11 +2718,11 @@
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
@@ -2617,108 +2737,776 @@
       <c r="S69" s="5"/>
       <c r="T69" s="5"/>
     </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="5"/>
+      <c r="P70" s="5"/>
+      <c r="Q70" s="5"/>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+      <c r="O71" s="5"/>
+      <c r="P71" s="5"/>
+      <c r="Q71" s="5"/>
+      <c r="R71" s="5"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="5"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
+      <c r="N72" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O72" s="5"/>
+      <c r="P72" s="5"/>
+      <c r="Q72" s="5"/>
+      <c r="R72" s="5"/>
+      <c r="S72" s="5"/>
+      <c r="T72" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="5"/>
+      <c r="O73" s="5"/>
+      <c r="P73" s="5"/>
+      <c r="Q73" s="5"/>
+      <c r="R73" s="5"/>
+      <c r="S73" s="5"/>
+      <c r="T73" s="5"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="5"/>
+      <c r="P74" s="5"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5"/>
+      <c r="S74" s="5"/>
+      <c r="T74" s="5"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5"/>
+      <c r="Q75" s="5"/>
+      <c r="R75" s="5"/>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
+      <c r="O77" s="5"/>
+      <c r="P77" s="5"/>
+      <c r="Q77" s="5"/>
+      <c r="R77" s="5"/>
+      <c r="S77" s="5"/>
+      <c r="T77" s="5"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+      <c r="O78" s="5"/>
+      <c r="P78" s="5"/>
+      <c r="Q78" s="5"/>
+      <c r="R78" s="5"/>
+      <c r="S78" s="5"/>
+      <c r="T78" s="5"/>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+      <c r="P79" s="5"/>
+      <c r="Q79" s="5"/>
+      <c r="R79" s="5"/>
+      <c r="S79" s="5"/>
+      <c r="T79" s="5"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="5"/>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="5"/>
+      <c r="R80" s="5"/>
+      <c r="S80" s="5"/>
+      <c r="T80" s="5"/>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5"/>
+      <c r="O81" s="5"/>
+      <c r="P81" s="5"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="5"/>
+      <c r="S81" s="5"/>
+      <c r="T81" s="5"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5"/>
+      <c r="O82" s="5"/>
+      <c r="P82" s="5"/>
+      <c r="Q82" s="5"/>
+      <c r="R82" s="5"/>
+      <c r="S82" s="5"/>
+      <c r="T82" s="5"/>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="5"/>
+      <c r="P83" s="5"/>
+      <c r="Q83" s="5"/>
+      <c r="R83" s="5"/>
+      <c r="S83" s="5"/>
+      <c r="T83" s="5"/>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="5"/>
+      <c r="O84" s="5"/>
+      <c r="P84" s="5"/>
+      <c r="Q84" s="5"/>
+      <c r="R84" s="5"/>
+      <c r="S84" s="5"/>
+      <c r="T84" s="5"/>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O85" s="5"/>
+      <c r="P85" s="5"/>
+      <c r="Q85" s="5"/>
+      <c r="R85" s="5"/>
+      <c r="S85" s="5"/>
+      <c r="T85" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="5"/>
+      <c r="N86" s="5"/>
+      <c r="O86" s="5"/>
+      <c r="P86" s="5"/>
+      <c r="Q86" s="5"/>
+      <c r="R86" s="5"/>
+      <c r="S86" s="5"/>
+      <c r="T86" s="5"/>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
+      <c r="O87" s="5"/>
+      <c r="P87" s="5"/>
+      <c r="Q87" s="5"/>
+      <c r="R87" s="5"/>
+      <c r="S87" s="5"/>
+      <c r="T87" s="5"/>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="5"/>
+      <c r="N88" s="5"/>
+      <c r="O88" s="5"/>
+      <c r="P88" s="5"/>
+      <c r="Q88" s="5"/>
+      <c r="R88" s="5"/>
+      <c r="S88" s="5"/>
+      <c r="T88" s="5"/>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="L89" s="5"/>
+      <c r="M89" s="5"/>
+      <c r="N89" s="5"/>
+      <c r="O89" s="5"/>
+      <c r="P89" s="5"/>
+      <c r="Q89" s="5"/>
+      <c r="R89" s="5"/>
+      <c r="S89" s="5"/>
+      <c r="T89" s="5"/>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
+      <c r="M90" s="5"/>
+      <c r="N90" s="5"/>
+      <c r="O90" s="5"/>
+      <c r="P90" s="5"/>
+      <c r="Q90" s="5"/>
+      <c r="R90" s="5"/>
+      <c r="S90" s="5"/>
+      <c r="T90" s="5"/>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5"/>
+      <c r="M91" s="5"/>
+      <c r="N91" s="5"/>
+      <c r="O91" s="5"/>
+      <c r="P91" s="5"/>
+      <c r="Q91" s="5"/>
+      <c r="R91" s="5"/>
+      <c r="S91" s="5"/>
+      <c r="T91" s="5"/>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="5"/>
+      <c r="N92" s="5"/>
+      <c r="O92" s="5"/>
+      <c r="P92" s="5"/>
+      <c r="Q92" s="5"/>
+      <c r="R92" s="5"/>
+      <c r="S92" s="5"/>
+      <c r="T92" s="5"/>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
+      <c r="M93" s="5"/>
+      <c r="N93" s="5"/>
+      <c r="O93" s="5"/>
+      <c r="P93" s="5"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="5"/>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="5"/>
+      <c r="N94" s="5"/>
+      <c r="O94" s="5"/>
+      <c r="P94" s="5"/>
+      <c r="Q94" s="5"/>
+      <c r="R94" s="5"/>
+      <c r="S94" s="5"/>
+      <c r="T94" s="5"/>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="5"/>
+      <c r="N95" s="5"/>
+      <c r="O95" s="5"/>
+      <c r="P95" s="5"/>
+      <c r="Q95" s="5"/>
+      <c r="R95" s="5"/>
+      <c r="S95" s="5"/>
+      <c r="T95" s="5"/>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5"/>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="5"/>
+      <c r="M96" s="5"/>
+      <c r="N96" s="5"/>
+      <c r="O96" s="5"/>
+      <c r="P96" s="5"/>
+      <c r="Q96" s="5"/>
+      <c r="R96" s="5"/>
+      <c r="S96" s="5"/>
+      <c r="T96" s="5"/>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5"/>
+      <c r="N97" s="5"/>
+      <c r="O97" s="5"/>
+      <c r="P97" s="5"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="5"/>
+      <c r="S97" s="5"/>
+      <c r="T97" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="79">
-    <mergeCell ref="T57:T69"/>
-    <mergeCell ref="T20:T31"/>
-    <mergeCell ref="N32:S44"/>
-    <mergeCell ref="T32:T44"/>
-    <mergeCell ref="N45:S56"/>
-    <mergeCell ref="T45:T56"/>
+  <mergeCells count="99">
+    <mergeCell ref="N72:S84"/>
+    <mergeCell ref="T72:T84"/>
+    <mergeCell ref="A85:A97"/>
+    <mergeCell ref="B85:B97"/>
+    <mergeCell ref="C85:G97"/>
+    <mergeCell ref="H85:J97"/>
+    <mergeCell ref="K85:M97"/>
+    <mergeCell ref="N85:S97"/>
+    <mergeCell ref="T85:T97"/>
+    <mergeCell ref="A72:A84"/>
+    <mergeCell ref="B72:B84"/>
+    <mergeCell ref="C72:G84"/>
+    <mergeCell ref="H72:J84"/>
+    <mergeCell ref="K72:M84"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="H34:J46"/>
+    <mergeCell ref="K34:M46"/>
+    <mergeCell ref="C34:G46"/>
+    <mergeCell ref="A20:R20"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A47:A58"/>
+    <mergeCell ref="B47:B58"/>
+    <mergeCell ref="C47:G58"/>
+    <mergeCell ref="H59:J71"/>
+    <mergeCell ref="K59:M71"/>
+    <mergeCell ref="C59:G71"/>
+    <mergeCell ref="A59:A71"/>
+    <mergeCell ref="B59:B71"/>
+    <mergeCell ref="H47:J58"/>
+    <mergeCell ref="K47:M58"/>
+    <mergeCell ref="A34:A46"/>
+    <mergeCell ref="B34:B46"/>
+    <mergeCell ref="N21:S21"/>
+    <mergeCell ref="N22:S33"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M33"/>
+    <mergeCell ref="H22:J33"/>
+    <mergeCell ref="A22:A33"/>
+    <mergeCell ref="B22:B33"/>
+    <mergeCell ref="C22:G33"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:R15"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:R13"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:R16"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="K17:R17"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:R14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K15:R15"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:R13"/>
-    <mergeCell ref="A32:A44"/>
-    <mergeCell ref="B32:B44"/>
-    <mergeCell ref="N19:S19"/>
-    <mergeCell ref="N20:S31"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:R18"/>
+    <mergeCell ref="C19:G19"/>
     <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M31"/>
-    <mergeCell ref="H20:J31"/>
-    <mergeCell ref="A20:A31"/>
-    <mergeCell ref="B20:B31"/>
-    <mergeCell ref="C20:G31"/>
-    <mergeCell ref="A45:A56"/>
-    <mergeCell ref="B45:B56"/>
-    <mergeCell ref="C45:G56"/>
-    <mergeCell ref="H57:J69"/>
-    <mergeCell ref="K57:M69"/>
-    <mergeCell ref="C57:G69"/>
-    <mergeCell ref="A57:A69"/>
-    <mergeCell ref="B57:B69"/>
-    <mergeCell ref="H45:J56"/>
-    <mergeCell ref="K45:M56"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="H32:J44"/>
-    <mergeCell ref="K32:M44"/>
-    <mergeCell ref="C32:G44"/>
-    <mergeCell ref="A18:R18"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="N57:S69"/>
+    <mergeCell ref="K19:R19"/>
+    <mergeCell ref="T59:T71"/>
+    <mergeCell ref="T22:T33"/>
+    <mergeCell ref="N34:S46"/>
+    <mergeCell ref="T34:T46"/>
+    <mergeCell ref="N47:S58"/>
+    <mergeCell ref="T47:T58"/>
+    <mergeCell ref="N59:S71"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
-    <hyperlink ref="C7" r:id="rId5"/>
-    <hyperlink ref="C8" r:id="rId6"/>
-    <hyperlink ref="C9" r:id="rId7"/>
-    <hyperlink ref="C10" r:id="rId8"/>
-    <hyperlink ref="C11" r:id="rId9"/>
-    <hyperlink ref="C12" r:id="rId10"/>
-    <hyperlink ref="C13" r:id="rId11"/>
-    <hyperlink ref="C14" r:id="rId12"/>
-    <hyperlink ref="C15" r:id="rId13"/>
-    <hyperlink ref="C16" r:id="rId14"/>
-    <hyperlink ref="C17" r:id="rId15"/>
-    <hyperlink ref="C20" r:id="rId16"/>
-    <hyperlink ref="C32" r:id="rId17"/>
-    <hyperlink ref="C45" r:id="rId18"/>
-    <hyperlink ref="C57" r:id="rId19"/>
+    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId4"/>
+    <hyperlink ref="C9" r:id="rId5"/>
+    <hyperlink ref="C10" r:id="rId6"/>
+    <hyperlink ref="C11" r:id="rId7"/>
+    <hyperlink ref="C12" r:id="rId8"/>
+    <hyperlink ref="C13" r:id="rId9"/>
+    <hyperlink ref="C14" r:id="rId10"/>
+    <hyperlink ref="C15" r:id="rId11"/>
+    <hyperlink ref="C16" r:id="rId12"/>
+    <hyperlink ref="C17" r:id="rId13"/>
+    <hyperlink ref="C18" r:id="rId14"/>
+    <hyperlink ref="C19" r:id="rId15"/>
+    <hyperlink ref="C22" r:id="rId16"/>
+    <hyperlink ref="C34" r:id="rId17"/>
+    <hyperlink ref="C47" r:id="rId18"/>
+    <hyperlink ref="C59" r:id="rId19"/>
+    <hyperlink ref="C72" r:id="rId20"/>
+    <hyperlink ref="C85" r:id="rId21"/>
+    <hyperlink ref="C5" r:id="rId22"/>
+    <hyperlink ref="C6" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cambios en ubicacion bus
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
   <si>
     <t>Recurso</t>
   </si>
@@ -541,6 +541,31 @@
   <si>
     <t>Obtiene el recorrido especificado por el parametro de la url.</t>
   </si>
+  <si>
+    <t>/colector/buses</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/colector/buses</t>
+  </si>
+  <si>
+    <t>{
+   "placa": "ZOE101",
+   "tde":"2016/10/16 13:13:00",
+      "coordenada":{
+   "latitud": "9.113633",
+   "longitud":"-72.114842"
+ } 
+}</t>
+  </si>
+  <si>
+    <t>no importa</t>
+  </si>
+  <si>
+    <t>recibe los buses y se encarga de crear un fichero con el nombre de la placa y el día en una carpeta llamada historico.</t>
+  </si>
+  <si>
+    <t>semi implementado</t>
+  </si>
 </sst>
 </file>
 
@@ -584,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -607,14 +632,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -946,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T97"/>
+  <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="I88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T98" sqref="T98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,15 +995,15 @@
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1190,11 +1218,11 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
       <c r="K8" s="5" t="s">
         <v>17</v>
       </c>
@@ -1223,11 +1251,11 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
       <c r="K9" s="5" t="s">
         <v>19</v>
       </c>
@@ -1256,11 +1284,11 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
       <c r="K10" s="5" t="s">
         <v>22</v>
       </c>
@@ -3381,60 +3409,72 @@
       <c r="S97" s="5"/>
       <c r="T97" s="5"/>
     </row>
+    <row r="98" spans="1:20" s="11" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="L98" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="N98" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="O98" s="5"/>
+      <c r="P98" s="5"/>
+      <c r="Q98" s="5"/>
+      <c r="R98" s="5"/>
+      <c r="S98" s="5"/>
+      <c r="T98" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="99">
-    <mergeCell ref="N72:S84"/>
-    <mergeCell ref="T72:T84"/>
-    <mergeCell ref="A85:A97"/>
-    <mergeCell ref="B85:B97"/>
-    <mergeCell ref="C85:G97"/>
-    <mergeCell ref="H85:J97"/>
-    <mergeCell ref="K85:M97"/>
-    <mergeCell ref="N85:S97"/>
-    <mergeCell ref="T85:T97"/>
-    <mergeCell ref="A72:A84"/>
-    <mergeCell ref="B72:B84"/>
-    <mergeCell ref="C72:G84"/>
-    <mergeCell ref="H72:J84"/>
-    <mergeCell ref="K72:M84"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="H34:J46"/>
-    <mergeCell ref="K34:M46"/>
-    <mergeCell ref="C34:G46"/>
-    <mergeCell ref="A20:R20"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="A47:A58"/>
-    <mergeCell ref="B47:B58"/>
-    <mergeCell ref="C47:G58"/>
-    <mergeCell ref="H59:J71"/>
-    <mergeCell ref="K59:M71"/>
-    <mergeCell ref="C59:G71"/>
-    <mergeCell ref="A59:A71"/>
-    <mergeCell ref="B59:B71"/>
-    <mergeCell ref="H47:J58"/>
-    <mergeCell ref="K47:M58"/>
-    <mergeCell ref="A34:A46"/>
-    <mergeCell ref="B34:B46"/>
-    <mergeCell ref="N21:S21"/>
-    <mergeCell ref="N22:S33"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K22:M33"/>
-    <mergeCell ref="H22:J33"/>
-    <mergeCell ref="A22:A33"/>
-    <mergeCell ref="B22:B33"/>
-    <mergeCell ref="C22:G33"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:J14"/>
+  <mergeCells count="102">
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:J98"/>
+    <mergeCell ref="N98:S98"/>
+    <mergeCell ref="K19:R19"/>
+    <mergeCell ref="T59:T71"/>
+    <mergeCell ref="T22:T33"/>
+    <mergeCell ref="N34:S46"/>
+    <mergeCell ref="T34:T46"/>
+    <mergeCell ref="N47:S58"/>
+    <mergeCell ref="T47:T58"/>
+    <mergeCell ref="N59:S71"/>
+    <mergeCell ref="K16:R16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:R18"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
     <mergeCell ref="K14:R14"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="H15:J15"/>
@@ -3451,37 +3491,62 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="H7:J7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="A22:A33"/>
+    <mergeCell ref="B22:B33"/>
+    <mergeCell ref="C22:G33"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H14:J14"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:R16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:R17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:R18"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:R19"/>
-    <mergeCell ref="T59:T71"/>
-    <mergeCell ref="T22:T33"/>
-    <mergeCell ref="N34:S46"/>
-    <mergeCell ref="T34:T46"/>
-    <mergeCell ref="N47:S58"/>
-    <mergeCell ref="T47:T58"/>
-    <mergeCell ref="N59:S71"/>
+    <mergeCell ref="B34:B46"/>
+    <mergeCell ref="N21:S21"/>
+    <mergeCell ref="N22:S33"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M33"/>
+    <mergeCell ref="H22:J33"/>
+    <mergeCell ref="A47:A58"/>
+    <mergeCell ref="B47:B58"/>
+    <mergeCell ref="C47:G58"/>
+    <mergeCell ref="H59:J71"/>
+    <mergeCell ref="K59:M71"/>
+    <mergeCell ref="C59:G71"/>
+    <mergeCell ref="A59:A71"/>
+    <mergeCell ref="B59:B71"/>
+    <mergeCell ref="H47:J58"/>
+    <mergeCell ref="K47:M58"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="H34:J46"/>
+    <mergeCell ref="K34:M46"/>
+    <mergeCell ref="C34:G46"/>
+    <mergeCell ref="A20:R20"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A34:A46"/>
+    <mergeCell ref="N72:S84"/>
+    <mergeCell ref="T72:T84"/>
+    <mergeCell ref="A85:A97"/>
+    <mergeCell ref="B85:B97"/>
+    <mergeCell ref="C85:G97"/>
+    <mergeCell ref="H85:J97"/>
+    <mergeCell ref="K85:M97"/>
+    <mergeCell ref="N85:S97"/>
+    <mergeCell ref="T85:T97"/>
+    <mergeCell ref="A72:A84"/>
+    <mergeCell ref="B72:B84"/>
+    <mergeCell ref="C72:G84"/>
+    <mergeCell ref="H72:J84"/>
+    <mergeCell ref="K72:M84"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -3507,6 +3572,7 @@
     <hyperlink ref="C85" r:id="rId21"/>
     <hyperlink ref="C5" r:id="rId22"/>
     <hyperlink ref="C6" r:id="rId23"/>
+    <hyperlink ref="C98" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se creo la base de datos colector y se almacenara informacion tan pronto como la envia un bus
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19980" windowHeight="8580" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19980" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Administacion" sheetId="1" r:id="rId1"/>
@@ -516,16 +516,6 @@
     <t>http://localhost:8080/cloudBRT/api/colector/buses</t>
   </si>
   <si>
-    <t>{
-   "placa": "ZOE101",
-   "tde":"2016/10/16 13:13:00",
-      "coordenada":{
-   "latitud": "9.113633",
-   "longitud":"-72.114842"
- } 
-}</t>
-  </si>
-  <si>
     <t>no importa</t>
   </si>
   <si>
@@ -568,6 +558,16 @@
   "TipoBus": "Articulado",
   "Estado": true,
   "Coordenada": "{"latitud":0.0,"longitud":0.0}"
+}</t>
+  </si>
+  <si>
+    <t>{
+   "Placa": "ZOE101",
+   "Tde":"2016/10/16 13:13:00",
+      "Coordenada":{
+   "Latitud": "9.113633",
+   "Longitud":"-72.114842"
+ } 
 }</t>
   </si>
 </sst>
@@ -986,20 +986,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:T98"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="50.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.25" customWidth="1"/>
+    <col min="9" max="9" width="11.375" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="18" max="18" width="32.7109375" customWidth="1"/>
-    <col min="19" max="19" width="52.85546875" customWidth="1"/>
-    <col min="20" max="20" width="19.7109375" customWidth="1"/>
+    <col min="18" max="18" width="32.75" customWidth="1"/>
+    <col min="19" max="19" width="52.875" customWidth="1"/>
+    <col min="20" max="20" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -1296,7 +1296,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -3447,7 +3447,6 @@
     <mergeCell ref="N59:S71"/>
     <mergeCell ref="H59:J71"/>
     <mergeCell ref="K59:M71"/>
-    <mergeCell ref="C11:G11"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="K11:R11"/>
     <mergeCell ref="C12:G12"/>
@@ -3494,6 +3493,7 @@
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="K10:R10"/>
+    <mergeCell ref="C11:G11"/>
     <mergeCell ref="K21:M21"/>
     <mergeCell ref="K22:M33"/>
     <mergeCell ref="H22:J33"/>
@@ -3574,8 +3574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3743,17 +3743,17 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="10" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
@@ -3761,16 +3761,11 @@
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
       <c r="T6" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:S5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="K6:M6"/>
     <mergeCell ref="K3:S3"/>
     <mergeCell ref="N6:S6"/>
     <mergeCell ref="C6:G6"/>
@@ -3780,6 +3775,11 @@
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="A4:R4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:S5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="K6:M6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>

</xml_diff>

<commit_message>
se creo base de datos de personas y transacciones de conductor para crear el servicio de crear conductor
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
   <si>
     <t>Recurso</t>
   </si>
@@ -597,6 +597,23 @@
   <si>
     <t>http://localhost:8080/cloudBRT/api/rutas/administracion/modificar/categoria</t>
   </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/conductor/administracion/crear</t>
+  </si>
+  <si>
+    <t>{
+ "Cedula":1098123764,
+"Primer Nombre":"Edilberto",
+"Segundo Nombre":"José",
+"Primer Apellido":"Guarin",
+"Segundo Apellido":"Santana",
+"Numero de Licencia":9344393,
+"Grupo Sanguineo":"O+"
+}</t>
+  </si>
+  <si>
+    <t>crea un conductor en la base de datos</t>
+  </si>
 </sst>
 </file>
 
@@ -640,7 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -670,18 +687,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1017,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T90"/>
+  <dimension ref="A1:T91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N92" sqref="N92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,15 +1059,15 @@
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1123,18 +1143,18 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="10" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
       <c r="K4" s="11" t="s">
         <v>24</v>
       </c>
@@ -1156,18 +1176,18 @@
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="10" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="11" t="s">
         <v>25</v>
       </c>
@@ -1189,18 +1209,18 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="10" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="11" t="s">
         <v>26</v>
       </c>
@@ -1222,18 +1242,18 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="10" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="11" t="s">
         <v>30</v>
       </c>
@@ -1255,18 +1275,18 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="10" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="11" t="s">
         <v>29</v>
       </c>
@@ -1288,18 +1308,18 @@
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="10" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
       <c r="K9" s="11" t="s">
         <v>28</v>
       </c>
@@ -1321,18 +1341,18 @@
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="10" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
       <c r="K10" s="11" t="s">
         <v>27</v>
       </c>
@@ -1354,18 +1374,18 @@
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="10" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
       <c r="K11" s="11" t="s">
         <v>57</v>
       </c>
@@ -1388,11 +1408,11 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
       <c r="K12" s="11" t="s">
         <v>4</v>
       </c>
@@ -1417,19 +1437,19 @@
       <c r="B13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>95</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10" t="s">
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12" t="s">
         <v>32</v>
       </c>
       <c r="L13" s="11"/>
@@ -1454,9 +1474,9 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
@@ -1476,9 +1496,9 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
@@ -1498,9 +1518,9 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
@@ -1520,9 +1540,9 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
@@ -1542,9 +1562,9 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
@@ -1564,9 +1584,9 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
@@ -1586,9 +1606,9 @@
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
@@ -1608,9 +1628,9 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
@@ -1630,9 +1650,9 @@
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
@@ -1652,9 +1672,9 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
@@ -1674,9 +1694,9 @@
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
@@ -1695,19 +1715,19 @@
       <c r="B25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="10" t="s">
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="12" t="s">
         <v>34</v>
       </c>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
-      <c r="K25" s="10" t="s">
+      <c r="K25" s="12" t="s">
         <v>32</v>
       </c>
       <c r="L25" s="11"/>
@@ -1727,11 +1747,11 @@
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -1749,11 +1769,11 @@
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
@@ -1771,11 +1791,11 @@
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
@@ -1793,11 +1813,11 @@
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
@@ -1815,11 +1835,11 @@
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
@@ -1837,11 +1857,11 @@
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
@@ -1859,11 +1879,11 @@
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
@@ -1881,11 +1901,11 @@
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
@@ -1903,11 +1923,11 @@
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
@@ -1925,11 +1945,11 @@
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
@@ -1947,11 +1967,11 @@
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
@@ -1969,11 +1989,11 @@
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
@@ -1995,19 +2015,19 @@
       <c r="B38" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="10" t="s">
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="12" t="s">
         <v>36</v>
       </c>
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="10" t="s">
+      <c r="K38" s="12" t="s">
         <v>32</v>
       </c>
       <c r="L38" s="11"/>
@@ -2027,11 +2047,11 @@
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="11"/>
@@ -2049,11 +2069,11 @@
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="11"/>
@@ -2071,11 +2091,11 @@
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="11"/>
@@ -2093,11 +2113,11 @@
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
       <c r="H42" s="11"/>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
@@ -2115,11 +2135,11 @@
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
@@ -2137,11 +2157,11 @@
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
@@ -2159,11 +2179,11 @@
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
@@ -2181,11 +2201,11 @@
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
@@ -2203,11 +2223,11 @@
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
       <c r="J47" s="11"/>
@@ -2225,11 +2245,11 @@
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
@@ -2247,11 +2267,11 @@
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
@@ -2273,19 +2293,19 @@
       <c r="B50" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="10" t="s">
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="12" t="s">
         <v>39</v>
       </c>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
-      <c r="K50" s="10" t="s">
+      <c r="K50" s="12" t="s">
         <v>32</v>
       </c>
       <c r="L50" s="11"/>
@@ -2305,11 +2325,11 @@
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
@@ -2327,11 +2347,11 @@
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
@@ -2349,11 +2369,11 @@
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
       <c r="J53" s="11"/>
@@ -2371,11 +2391,11 @@
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
@@ -2393,11 +2413,11 @@
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
       <c r="J55" s="11"/>
@@ -2415,11 +2435,11 @@
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
       <c r="B56" s="11"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
@@ -2437,11 +2457,11 @@
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="B57" s="11"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
@@ -2459,11 +2479,11 @@
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
       <c r="H58" s="11"/>
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
@@ -2481,11 +2501,11 @@
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="11"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
       <c r="H59" s="11"/>
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
@@ -2503,11 +2523,11 @@
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="11"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
@@ -2525,11 +2545,11 @@
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="11"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
       <c r="H61" s="11"/>
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
@@ -2547,11 +2567,11 @@
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="11"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
       <c r="H62" s="11"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
@@ -2573,19 +2593,19 @@
       <c r="B63" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="10" t="s">
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="12" t="s">
         <v>41</v>
       </c>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
-      <c r="K63" s="10" t="s">
+      <c r="K63" s="12" t="s">
         <v>32</v>
       </c>
       <c r="L63" s="11"/>
@@ -2605,11 +2625,11 @@
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="11"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
       <c r="H64" s="11"/>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
@@ -2627,11 +2647,11 @@
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="11"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
       <c r="H65" s="11"/>
       <c r="I65" s="11"/>
       <c r="J65" s="11"/>
@@ -2649,11 +2669,11 @@
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="11"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
       <c r="J66" s="11"/>
@@ -2671,11 +2691,11 @@
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
       <c r="H67" s="11"/>
       <c r="I67" s="11"/>
       <c r="J67" s="11"/>
@@ -2693,11 +2713,11 @@
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="11"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
       <c r="J68" s="11"/>
@@ -2715,11 +2735,11 @@
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="11"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
       <c r="H69" s="11"/>
       <c r="I69" s="11"/>
       <c r="J69" s="11"/>
@@ -2737,11 +2757,11 @@
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="11"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
       <c r="J70" s="11"/>
@@ -2759,11 +2779,11 @@
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
       <c r="J71" s="11"/>
@@ -2781,11 +2801,11 @@
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="11"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
       <c r="J72" s="11"/>
@@ -2803,11 +2823,11 @@
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="11"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
       <c r="H73" s="11"/>
       <c r="I73" s="11"/>
       <c r="J73" s="11"/>
@@ -2825,11 +2845,11 @@
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="11"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
       <c r="H74" s="11"/>
       <c r="I74" s="11"/>
       <c r="J74" s="11"/>
@@ -2847,11 +2867,11 @@
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="11"/>
       <c r="B75" s="11"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
       <c r="H75" s="11"/>
       <c r="I75" s="11"/>
       <c r="J75" s="11"/>
@@ -2873,19 +2893,19 @@
       <c r="B76" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C76" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="10" t="s">
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="12" t="s">
         <v>42</v>
       </c>
       <c r="I76" s="11"/>
       <c r="J76" s="11"/>
-      <c r="K76" s="10" t="s">
+      <c r="K76" s="12" t="s">
         <v>32</v>
       </c>
       <c r="L76" s="11"/>
@@ -2905,11 +2925,11 @@
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="11"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
       <c r="H77" s="11"/>
       <c r="I77" s="11"/>
       <c r="J77" s="11"/>
@@ -2927,11 +2947,11 @@
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="11"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11"/>
       <c r="J78" s="11"/>
@@ -2949,11 +2969,11 @@
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
       <c r="J79" s="11"/>
@@ -2971,11 +2991,11 @@
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="11"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
       <c r="H80" s="11"/>
       <c r="I80" s="11"/>
       <c r="J80" s="11"/>
@@ -2993,11 +3013,11 @@
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="11"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
       <c r="H81" s="11"/>
       <c r="I81" s="11"/>
       <c r="J81" s="11"/>
@@ -3015,11 +3035,11 @@
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="11"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
       <c r="H82" s="11"/>
       <c r="I82" s="11"/>
       <c r="J82" s="11"/>
@@ -3037,11 +3057,11 @@
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="11"/>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
       <c r="H83" s="11"/>
       <c r="I83" s="11"/>
       <c r="J83" s="11"/>
@@ -3059,11 +3079,11 @@
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="11"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
       <c r="H84" s="11"/>
       <c r="I84" s="11"/>
       <c r="J84" s="11"/>
@@ -3081,11 +3101,11 @@
     <row r="85" spans="1:20" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="11"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
-      <c r="G85" s="12"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
       <c r="H85" s="11"/>
       <c r="I85" s="11"/>
       <c r="J85" s="11"/>
@@ -3103,11 +3123,11 @@
     <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
       <c r="B86" s="11"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
       <c r="H86" s="11"/>
       <c r="I86" s="11"/>
       <c r="J86" s="11"/>
@@ -3125,11 +3145,11 @@
     <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11"/>
       <c r="B87" s="11"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="12"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11"/>
       <c r="J87" s="11"/>
@@ -3147,11 +3167,11 @@
     <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
       <c r="B88" s="11"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="12"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
       <c r="H88" s="11"/>
       <c r="I88" s="11"/>
       <c r="J88" s="11"/>
@@ -3173,19 +3193,19 @@
       <c r="B89" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="12" t="s">
+      <c r="C89" s="13" t="s">
         <v>108</v>
       </c>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
-      <c r="H89" s="10" t="s">
+      <c r="H89" s="12" t="s">
         <v>58</v>
       </c>
       <c r="I89" s="11"/>
       <c r="J89" s="11"/>
-      <c r="K89" s="10" t="s">
+      <c r="K89" s="12" t="s">
         <v>32</v>
       </c>
       <c r="L89" s="11"/>
@@ -3209,19 +3229,19 @@
       <c r="B90" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C90" s="12" t="s">
+      <c r="C90" s="13" t="s">
         <v>109</v>
       </c>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
-      <c r="H90" s="10" t="s">
+      <c r="H90" s="12" t="s">
         <v>58</v>
       </c>
       <c r="I90" s="11"/>
       <c r="J90" s="11"/>
-      <c r="K90" s="10" t="s">
+      <c r="K90" s="12" t="s">
         <v>32</v>
       </c>
       <c r="L90" s="11"/>
@@ -3238,73 +3258,49 @@
         <v>60</v>
       </c>
     </row>
+    <row r="91" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="I91" s="11"/>
+      <c r="J91" s="11"/>
+      <c r="K91" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L91" s="11"/>
+      <c r="M91" s="11"/>
+      <c r="N91" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="O91" s="11"/>
+      <c r="P91" s="11"/>
+      <c r="Q91" s="11"/>
+      <c r="R91" s="11"/>
+      <c r="S91" s="11"/>
+      <c r="T91" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="82">
-    <mergeCell ref="T13:T24"/>
-    <mergeCell ref="N25:S37"/>
-    <mergeCell ref="T25:T37"/>
-    <mergeCell ref="N38:S49"/>
-    <mergeCell ref="T38:T49"/>
-    <mergeCell ref="N50:S62"/>
-    <mergeCell ref="H50:J62"/>
-    <mergeCell ref="K50:M62"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="C50:G62"/>
-    <mergeCell ref="N63:S75"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="H13:J24"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="C38:G49"/>
-    <mergeCell ref="A13:A24"/>
-    <mergeCell ref="B13:B24"/>
-    <mergeCell ref="C13:G24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H38:J49"/>
-    <mergeCell ref="K38:M49"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="H25:J37"/>
-    <mergeCell ref="K25:M37"/>
-    <mergeCell ref="C25:G37"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A25:A37"/>
-    <mergeCell ref="B25:B37"/>
-    <mergeCell ref="N12:S12"/>
-    <mergeCell ref="N13:S24"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M24"/>
-    <mergeCell ref="T76:T88"/>
-    <mergeCell ref="A63:A75"/>
-    <mergeCell ref="B63:B75"/>
-    <mergeCell ref="C63:G75"/>
-    <mergeCell ref="H63:J75"/>
-    <mergeCell ref="K63:M75"/>
-    <mergeCell ref="T63:T75"/>
+  <mergeCells count="86">
+    <mergeCell ref="N89:S89"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="N91:S91"/>
     <mergeCell ref="A50:A62"/>
     <mergeCell ref="B50:B62"/>
     <mergeCell ref="T50:T62"/>
@@ -3321,7 +3317,71 @@
     <mergeCell ref="N76:S88"/>
     <mergeCell ref="C89:G89"/>
     <mergeCell ref="H89:J89"/>
-    <mergeCell ref="N89:S89"/>
+    <mergeCell ref="T76:T88"/>
+    <mergeCell ref="A63:A75"/>
+    <mergeCell ref="B63:B75"/>
+    <mergeCell ref="C63:G75"/>
+    <mergeCell ref="H63:J75"/>
+    <mergeCell ref="K63:M75"/>
+    <mergeCell ref="T63:T75"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="H25:J37"/>
+    <mergeCell ref="K25:M37"/>
+    <mergeCell ref="C25:G37"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A25:A37"/>
+    <mergeCell ref="B25:B37"/>
+    <mergeCell ref="N12:S12"/>
+    <mergeCell ref="N13:S24"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M24"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H38:J49"/>
+    <mergeCell ref="K38:M49"/>
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="C38:G49"/>
+    <mergeCell ref="A13:A24"/>
+    <mergeCell ref="B13:B24"/>
+    <mergeCell ref="C13:G24"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="N63:S75"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H13:J24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="N50:S62"/>
+    <mergeCell ref="H50:J62"/>
+    <mergeCell ref="K50:M62"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="C50:G62"/>
+    <mergeCell ref="T13:T24"/>
+    <mergeCell ref="N25:S37"/>
+    <mergeCell ref="T25:T37"/>
+    <mergeCell ref="N38:S49"/>
+    <mergeCell ref="T38:T49"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -3341,6 +3401,7 @@
     <hyperlink ref="C89" r:id="rId15"/>
     <hyperlink ref="C90" r:id="rId16"/>
     <hyperlink ref="C4" r:id="rId17"/>
+    <hyperlink ref="C91" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3366,15 +3427,15 @@
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -3475,18 +3536,18 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="10" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="11" t="s">
         <v>4</v>
       </c>
@@ -3511,14 +3572,14 @@
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>50</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I6" s="11"/>
@@ -3569,7 +3630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S16"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -3586,18 +3647,18 @@
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="10" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="11" t="s">
         <v>14</v>
       </c>
@@ -3619,18 +3680,18 @@
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="15" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="11" t="s">
         <v>20</v>
       </c>
@@ -3652,18 +3713,18 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="15" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
       <c r="K6" s="11" t="s">
         <v>16</v>
       </c>
@@ -3685,18 +3746,18 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="10" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="11" t="s">
         <v>22</v>
       </c>
@@ -3718,18 +3779,18 @@
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="10" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
       <c r="K10" s="11" t="s">
         <v>46</v>
       </c>
@@ -3751,18 +3812,18 @@
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="10" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
       <c r="K12" s="11" t="s">
         <v>48</v>
       </c>
@@ -3784,18 +3845,18 @@
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="10" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
       <c r="K14" s="11" t="s">
         <v>13</v>
       </c>
@@ -3817,18 +3878,18 @@
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="15" t="s">
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="11" t="s">
         <v>18</v>
       </c>
@@ -3845,30 +3906,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="K14:R14"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:R16"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
cambios generales, refactor de uris, creacion de metodos modificar y eliminar para los TConductor
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="114">
   <si>
     <t>Recurso</t>
   </si>
@@ -613,6 +613,12 @@
   </si>
   <si>
     <t>crea un conductor en la base de datos</t>
+  </si>
+  <si>
+    <t>{
+  "Ruta":"p8",
+  "Categoria": "Ruta de la Excelencia"
+}</t>
   </si>
 </sst>
 </file>
@@ -692,16 +698,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1039,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N92" sqref="N92"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90:J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,15 +1065,15 @@
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1081,26 +1087,26 @@
       <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1110,28 +1116,28 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
       <c r="S3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1143,18 +1149,18 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="12" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="11" t="s">
         <v>24</v>
       </c>
@@ -1176,18 +1182,18 @@
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="12" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
       <c r="K5" s="11" t="s">
         <v>25</v>
       </c>
@@ -1209,18 +1215,18 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="12" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
       <c r="K6" s="11" t="s">
         <v>26</v>
       </c>
@@ -1242,18 +1248,18 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="12" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="11" t="s">
         <v>30</v>
       </c>
@@ -1275,18 +1281,18 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="12" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="11" t="s">
         <v>29</v>
       </c>
@@ -1308,18 +1314,18 @@
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="12" t="s">
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
       <c r="K9" s="11" t="s">
         <v>28</v>
       </c>
@@ -1341,18 +1347,18 @@
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="12" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="11" t="s">
         <v>27</v>
       </c>
@@ -1374,18 +1380,18 @@
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="12" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
       <c r="K11" s="11" t="s">
         <v>57</v>
       </c>
@@ -1408,11 +1414,11 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="11" t="s">
         <v>4</v>
       </c>
@@ -1437,19 +1443,19 @@
       <c r="B13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>95</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12" t="s">
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13" t="s">
         <v>32</v>
       </c>
       <c r="L13" s="11"/>
@@ -1474,9 +1480,9 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
@@ -1496,9 +1502,9 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
@@ -1518,9 +1524,9 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
@@ -1540,9 +1546,9 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
@@ -1562,9 +1568,9 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
@@ -1584,9 +1590,9 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
@@ -1606,9 +1612,9 @@
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
@@ -1628,9 +1634,9 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
@@ -1650,9 +1656,9 @@
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
@@ -1672,9 +1678,9 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
@@ -1694,9 +1700,9 @@
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
@@ -1715,19 +1721,19 @@
       <c r="B25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="12" t="s">
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13" t="s">
         <v>34</v>
       </c>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
-      <c r="K25" s="12" t="s">
+      <c r="K25" s="13" t="s">
         <v>32</v>
       </c>
       <c r="L25" s="11"/>
@@ -1747,11 +1753,11 @@
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -1769,11 +1775,11 @@
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
@@ -1791,11 +1797,11 @@
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
@@ -1813,11 +1819,11 @@
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
@@ -1835,11 +1841,11 @@
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
@@ -1857,11 +1863,11 @@
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
@@ -1879,11 +1885,11 @@
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
@@ -1901,11 +1907,11 @@
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
@@ -1923,11 +1929,11 @@
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
@@ -1945,11 +1951,11 @@
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
@@ -1967,11 +1973,11 @@
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
@@ -1989,11 +1995,11 @@
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
@@ -2015,19 +2021,19 @@
       <c r="B38" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="12" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="12" t="s">
+      <c r="K38" s="13" t="s">
         <v>32</v>
       </c>
       <c r="L38" s="11"/>
@@ -2047,11 +2053,11 @@
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="11"/>
@@ -2069,11 +2075,11 @@
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="11"/>
@@ -2091,11 +2097,11 @@
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="11"/>
@@ -2113,11 +2119,11 @@
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
       <c r="H42" s="11"/>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
@@ -2135,11 +2141,11 @@
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
@@ -2157,11 +2163,11 @@
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
@@ -2179,11 +2185,11 @@
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
@@ -2201,11 +2207,11 @@
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
@@ -2223,11 +2229,11 @@
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
       <c r="J47" s="11"/>
@@ -2245,11 +2251,11 @@
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
@@ -2267,11 +2273,11 @@
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
@@ -2293,19 +2299,19 @@
       <c r="B50" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="12" t="s">
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="13" t="s">
         <v>39</v>
       </c>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
-      <c r="K50" s="12" t="s">
+      <c r="K50" s="13" t="s">
         <v>32</v>
       </c>
       <c r="L50" s="11"/>
@@ -2325,11 +2331,11 @@
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="11"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
@@ -2347,11 +2353,11 @@
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
@@ -2369,11 +2375,11 @@
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="11"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
       <c r="J53" s="11"/>
@@ -2391,11 +2397,11 @@
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
@@ -2413,11 +2419,11 @@
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
       <c r="J55" s="11"/>
@@ -2435,11 +2441,11 @@
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
       <c r="B56" s="11"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
@@ -2457,11 +2463,11 @@
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="B57" s="11"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
@@ -2479,11 +2485,11 @@
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
       <c r="H58" s="11"/>
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
@@ -2501,11 +2507,11 @@
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="11"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
       <c r="H59" s="11"/>
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
@@ -2523,11 +2529,11 @@
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="11"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
@@ -2545,11 +2551,11 @@
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="11"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
       <c r="H61" s="11"/>
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
@@ -2567,11 +2573,11 @@
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="11"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
       <c r="H62" s="11"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
@@ -2593,19 +2599,19 @@
       <c r="B63" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="12" t="s">
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="13" t="s">
         <v>41</v>
       </c>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
-      <c r="K63" s="12" t="s">
+      <c r="K63" s="13" t="s">
         <v>32</v>
       </c>
       <c r="L63" s="11"/>
@@ -2625,11 +2631,11 @@
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="11"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
       <c r="H64" s="11"/>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
@@ -2647,11 +2653,11 @@
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="11"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
       <c r="H65" s="11"/>
       <c r="I65" s="11"/>
       <c r="J65" s="11"/>
@@ -2669,11 +2675,11 @@
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="11"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
       <c r="J66" s="11"/>
@@ -2691,11 +2697,11 @@
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="11"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
       <c r="H67" s="11"/>
       <c r="I67" s="11"/>
       <c r="J67" s="11"/>
@@ -2713,11 +2719,11 @@
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="11"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
       <c r="J68" s="11"/>
@@ -2735,11 +2741,11 @@
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="11"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
       <c r="H69" s="11"/>
       <c r="I69" s="11"/>
       <c r="J69" s="11"/>
@@ -2757,11 +2763,11 @@
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="11"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
       <c r="J70" s="11"/>
@@ -2779,11 +2785,11 @@
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="13"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
       <c r="J71" s="11"/>
@@ -2801,11 +2807,11 @@
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="11"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
       <c r="J72" s="11"/>
@@ -2823,11 +2829,11 @@
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="11"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
       <c r="H73" s="11"/>
       <c r="I73" s="11"/>
       <c r="J73" s="11"/>
@@ -2845,11 +2851,11 @@
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="11"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
       <c r="H74" s="11"/>
       <c r="I74" s="11"/>
       <c r="J74" s="11"/>
@@ -2867,11 +2873,11 @@
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="11"/>
       <c r="B75" s="11"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
       <c r="H75" s="11"/>
       <c r="I75" s="11"/>
       <c r="J75" s="11"/>
@@ -2893,19 +2899,19 @@
       <c r="B76" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="12" t="s">
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="13" t="s">
         <v>42</v>
       </c>
       <c r="I76" s="11"/>
       <c r="J76" s="11"/>
-      <c r="K76" s="12" t="s">
+      <c r="K76" s="13" t="s">
         <v>32</v>
       </c>
       <c r="L76" s="11"/>
@@ -2925,11 +2931,11 @@
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="11"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
       <c r="H77" s="11"/>
       <c r="I77" s="11"/>
       <c r="J77" s="11"/>
@@ -2947,11 +2953,11 @@
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="11"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11"/>
       <c r="J78" s="11"/>
@@ -2969,11 +2975,11 @@
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
       <c r="J79" s="11"/>
@@ -2991,11 +2997,11 @@
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="11"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
       <c r="H80" s="11"/>
       <c r="I80" s="11"/>
       <c r="J80" s="11"/>
@@ -3013,11 +3019,11 @@
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="11"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
       <c r="H81" s="11"/>
       <c r="I81" s="11"/>
       <c r="J81" s="11"/>
@@ -3035,11 +3041,11 @@
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="11"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
       <c r="H82" s="11"/>
       <c r="I82" s="11"/>
       <c r="J82" s="11"/>
@@ -3057,11 +3063,11 @@
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="11"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
       <c r="H83" s="11"/>
       <c r="I83" s="11"/>
       <c r="J83" s="11"/>
@@ -3079,11 +3085,11 @@
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="11"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
       <c r="H84" s="11"/>
       <c r="I84" s="11"/>
       <c r="J84" s="11"/>
@@ -3101,11 +3107,11 @@
     <row r="85" spans="1:20" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="11"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
       <c r="H85" s="11"/>
       <c r="I85" s="11"/>
       <c r="J85" s="11"/>
@@ -3123,11 +3129,11 @@
     <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
       <c r="B86" s="11"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
       <c r="H86" s="11"/>
       <c r="I86" s="11"/>
       <c r="J86" s="11"/>
@@ -3145,11 +3151,11 @@
     <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11"/>
       <c r="B87" s="11"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11"/>
       <c r="J87" s="11"/>
@@ -3167,11 +3173,11 @@
     <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
       <c r="B88" s="11"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
       <c r="H88" s="11"/>
       <c r="I88" s="11"/>
       <c r="J88" s="11"/>
@@ -3193,19 +3199,19 @@
       <c r="B89" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C89" s="12" t="s">
         <v>108</v>
       </c>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
-      <c r="H89" s="12" t="s">
+      <c r="H89" s="13" t="s">
         <v>58</v>
       </c>
       <c r="I89" s="11"/>
       <c r="J89" s="11"/>
-      <c r="K89" s="12" t="s">
+      <c r="K89" s="13" t="s">
         <v>32</v>
       </c>
       <c r="L89" s="11"/>
@@ -3229,19 +3235,19 @@
       <c r="B90" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C90" s="12" t="s">
         <v>109</v>
       </c>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
-      <c r="H90" s="12" t="s">
-        <v>58</v>
+      <c r="H90" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="I90" s="11"/>
       <c r="J90" s="11"/>
-      <c r="K90" s="12" t="s">
+      <c r="K90" s="13" t="s">
         <v>32</v>
       </c>
       <c r="L90" s="11"/>
@@ -3265,19 +3271,19 @@
       <c r="B91" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C91" s="12" t="s">
         <v>110</v>
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
       <c r="G91" s="11"/>
-      <c r="H91" s="12" t="s">
+      <c r="H91" s="13" t="s">
         <v>111</v>
       </c>
       <c r="I91" s="11"/>
       <c r="J91" s="11"/>
-      <c r="K91" s="12" t="s">
+      <c r="K91" s="13" t="s">
         <v>32</v>
       </c>
       <c r="L91" s="11"/>
@@ -3296,11 +3302,71 @@
     </row>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="N89:S89"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="H91:J91"/>
-    <mergeCell ref="K91:M91"/>
-    <mergeCell ref="N91:S91"/>
+    <mergeCell ref="T13:T24"/>
+    <mergeCell ref="N25:S37"/>
+    <mergeCell ref="T25:T37"/>
+    <mergeCell ref="N38:S49"/>
+    <mergeCell ref="T38:T49"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H13:J24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="N50:S62"/>
+    <mergeCell ref="H50:J62"/>
+    <mergeCell ref="K50:M62"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="C50:G62"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="B13:B24"/>
+    <mergeCell ref="C13:G24"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="H38:J49"/>
+    <mergeCell ref="K38:M49"/>
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="C38:G49"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="H25:J37"/>
+    <mergeCell ref="K25:M37"/>
+    <mergeCell ref="C25:G37"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A25:A37"/>
+    <mergeCell ref="B25:B37"/>
+    <mergeCell ref="N12:S12"/>
+    <mergeCell ref="N13:S24"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M24"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="A13:A24"/>
+    <mergeCell ref="T76:T88"/>
+    <mergeCell ref="A63:A75"/>
+    <mergeCell ref="B63:B75"/>
+    <mergeCell ref="C63:G75"/>
+    <mergeCell ref="H63:J75"/>
+    <mergeCell ref="K63:M75"/>
+    <mergeCell ref="T63:T75"/>
+    <mergeCell ref="N63:S75"/>
     <mergeCell ref="A50:A62"/>
     <mergeCell ref="B50:B62"/>
     <mergeCell ref="T50:T62"/>
@@ -3317,71 +3383,11 @@
     <mergeCell ref="N76:S88"/>
     <mergeCell ref="C89:G89"/>
     <mergeCell ref="H89:J89"/>
-    <mergeCell ref="T76:T88"/>
-    <mergeCell ref="A63:A75"/>
-    <mergeCell ref="B63:B75"/>
-    <mergeCell ref="C63:G75"/>
-    <mergeCell ref="H63:J75"/>
-    <mergeCell ref="K63:M75"/>
-    <mergeCell ref="T63:T75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="H25:J37"/>
-    <mergeCell ref="K25:M37"/>
-    <mergeCell ref="C25:G37"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A25:A37"/>
-    <mergeCell ref="B25:B37"/>
-    <mergeCell ref="N12:S12"/>
-    <mergeCell ref="N13:S24"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M24"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H38:J49"/>
-    <mergeCell ref="K38:M49"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="C38:G49"/>
-    <mergeCell ref="A13:A24"/>
-    <mergeCell ref="B13:B24"/>
-    <mergeCell ref="C13:G24"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="N63:S75"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H13:J24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="N50:S62"/>
-    <mergeCell ref="H50:J62"/>
-    <mergeCell ref="K50:M62"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="C50:G62"/>
-    <mergeCell ref="T13:T24"/>
-    <mergeCell ref="N25:S37"/>
-    <mergeCell ref="T25:T37"/>
-    <mergeCell ref="N38:S49"/>
-    <mergeCell ref="T38:T49"/>
+    <mergeCell ref="N89:S89"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="N91:S91"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -3427,15 +3433,15 @@
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -3450,26 +3456,26 @@
       <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -3479,29 +3485,29 @@
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
       <c r="T3" s="6" t="s">
         <v>19</v>
       </c>
@@ -3536,18 +3542,18 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="12" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
       <c r="K5" s="11" t="s">
         <v>4</v>
       </c>
@@ -3572,14 +3578,14 @@
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>50</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="13" t="s">
         <v>56</v>
       </c>
       <c r="I6" s="11"/>
@@ -3647,18 +3653,18 @@
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="12" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="11" t="s">
         <v>14</v>
       </c>
@@ -3680,13 +3686,13 @@
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="16" t="s">
         <v>55</v>
       </c>
@@ -3713,13 +3719,13 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="16" t="s">
         <v>15</v>
       </c>
@@ -3746,18 +3752,18 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="12" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="11" t="s">
         <v>22</v>
       </c>
@@ -3779,18 +3785,18 @@
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="12" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="11" t="s">
         <v>46</v>
       </c>
@@ -3812,18 +3818,18 @@
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="12" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="11" t="s">
         <v>48</v>
       </c>
@@ -3845,18 +3851,18 @@
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="12" t="s">
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
       <c r="K14" s="11" t="s">
         <v>13</v>
       </c>
@@ -3878,13 +3884,13 @@
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="16" t="s">
         <v>17</v>
       </c>
@@ -3906,30 +3912,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:R16"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:R8"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:R2"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:R4"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:R14"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:R16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementacion del servicio que busca por ruta los itinerarios
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="153">
   <si>
     <t>Recurso</t>
   </si>
@@ -941,6 +941,59 @@
   <si>
     <t>Devuelve el tiempo teorico que tarda el bus en llegar a cada parada y el tiempo hasta donde esta tomando una velocidad de referencia.</t>
   </si>
+  <si>
+    <t>itinerario/tiempos/ruta/{$ruta}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/monitoreo/itinerario/tiempos/ruta/T3</t>
+  </si>
+  <si>
+    <t>{
+  "I2T3": {
+    "horario": {
+      "ST1": "00:00:00",
+      "ST2": "00:02:48",
+      "ST3": "00:07:55",
+      "ST4": "00:10:26",
+      "ST5": "00:15:12"
+    },
+    "avanceBus": "232:30:33"
+  },
+  "I1T3": {
+    "horario": {
+      "ST1": "00:00:00",
+      "ST2": "00:02:48",
+      "ST3": "00:07:55",
+      "ST4": "00:10:26",
+      "ST5": "00:15:12"
+    },
+    "avanceBus": "232:30:33"
+  },
+  "I4T3": {
+    "horario": {
+      "ST1": "00:00:00",
+      "ST2": "00:02:48",
+      "ST3": "00:07:55",
+      "ST4": "00:10:26",
+      "ST5": "00:15:12"
+    },
+    "avanceBus": "232:30:33"
+  },
+  "I3T3": {
+    "horario": {
+      "ST1": "00:00:00",
+      "ST2": "00:02:48",
+      "ST3": "00:07:55",
+      "ST4": "00:10:26",
+      "ST5": "00:15:12"
+    },
+    "avanceBus": "232:30:33"
+  }
+}</t>
+  </si>
+  <si>
+    <t>Devuelve el tiempo teorico que tarda el bus en llegar a cada parada y el tiempo hasta donde esta tomando una velocidad de referencia de todos los itinerarios que contengan la ruta especificada</t>
+  </si>
 </sst>
 </file>
 
@@ -984,7 +1037,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1031,10 +1084,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1401,15 +1457,15 @@
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1423,26 +1479,26 @@
       <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1452,28 +1508,28 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20" t="s">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
       <c r="S3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1485,18 +1541,18 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="18" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
       <c r="K4" s="17" t="s">
         <v>23</v>
       </c>
@@ -1518,18 +1574,18 @@
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="18" t="s">
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
       <c r="K5" s="17" t="s">
         <v>24</v>
       </c>
@@ -1551,18 +1607,18 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="18" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="17" t="s">
         <v>25</v>
       </c>
@@ -1584,18 +1640,18 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="18" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
       <c r="K7" s="17" t="s">
         <v>29</v>
       </c>
@@ -1617,18 +1673,18 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="18" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
       <c r="K8" s="17" t="s">
         <v>28</v>
       </c>
@@ -1650,18 +1706,18 @@
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="18" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
       <c r="K9" s="17" t="s">
         <v>27</v>
       </c>
@@ -1683,18 +1739,18 @@
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="18" t="s">
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
       <c r="K10" s="17" t="s">
         <v>26</v>
       </c>
@@ -1716,18 +1772,18 @@
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="18" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
       <c r="K11" s="17" t="s">
         <v>54</v>
       </c>
@@ -1749,18 +1805,18 @@
       <c r="B12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="18" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="17" t="s">
         <v>129</v>
       </c>
@@ -1782,18 +1838,18 @@
       <c r="B13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="18" t="s">
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
       <c r="K13" s="17" t="s">
         <v>132</v>
       </c>
@@ -1816,11 +1872,11 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
       <c r="K14" s="17" t="s">
         <v>4</v>
       </c>
@@ -1845,19 +1901,19 @@
       <c r="B15" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="18" t="s">
         <v>87</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18" t="s">
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L15" s="17"/>
@@ -1882,9 +1938,9 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
@@ -1904,9 +1960,9 @@
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
@@ -1926,9 +1982,9 @@
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
@@ -1948,9 +2004,9 @@
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
@@ -1970,9 +2026,9 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
@@ -1992,9 +2048,9 @@
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
@@ -2014,9 +2070,9 @@
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
@@ -2036,9 +2092,9 @@
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
@@ -2058,9 +2114,9 @@
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
       <c r="M24" s="17"/>
@@ -2080,9 +2136,9 @@
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
       <c r="M25" s="17"/>
@@ -2102,9 +2158,9 @@
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
@@ -2123,19 +2179,19 @@
       <c r="B27" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="18" t="s">
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19" t="s">
         <v>32</v>
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L27" s="17"/>
@@ -2155,11 +2211,11 @@
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="17"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
@@ -2177,11 +2233,11 @@
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
@@ -2199,11 +2255,11 @@
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="17"/>
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
@@ -2221,11 +2277,11 @@
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
@@ -2243,11 +2299,11 @@
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
       <c r="J32" s="17"/>
@@ -2265,11 +2321,11 @@
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="17"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="17"/>
       <c r="I33" s="17"/>
       <c r="J33" s="17"/>
@@ -2287,11 +2343,11 @@
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" s="17"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="17"/>
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
@@ -2309,11 +2365,11 @@
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
@@ -2331,11 +2387,11 @@
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="B36" s="17"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="17"/>
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
@@ -2353,11 +2409,11 @@
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="17"/>
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
@@ -2375,11 +2431,11 @@
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
@@ -2397,11 +2453,11 @@
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
       <c r="J39" s="17"/>
@@ -2423,19 +2479,19 @@
       <c r="B40" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="18" t="s">
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="19" t="s">
         <v>34</v>
       </c>
       <c r="I40" s="17"/>
       <c r="J40" s="17"/>
-      <c r="K40" s="18" t="s">
+      <c r="K40" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L40" s="17"/>
@@ -2455,11 +2511,11 @@
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
@@ -2477,11 +2533,11 @@
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
       <c r="B42" s="17"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
@@ -2499,11 +2555,11 @@
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
@@ -2521,11 +2577,11 @@
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
       <c r="B44" s="17"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
       <c r="H44" s="17"/>
       <c r="I44" s="17"/>
       <c r="J44" s="17"/>
@@ -2543,11 +2599,11 @@
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="17"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
       <c r="H45" s="17"/>
       <c r="I45" s="17"/>
       <c r="J45" s="17"/>
@@ -2565,11 +2621,11 @@
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
       <c r="B46" s="17"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
       <c r="H46" s="17"/>
       <c r="I46" s="17"/>
       <c r="J46" s="17"/>
@@ -2587,11 +2643,11 @@
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
       <c r="H47" s="17"/>
       <c r="I47" s="17"/>
       <c r="J47" s="17"/>
@@ -2609,11 +2665,11 @@
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
       <c r="H48" s="17"/>
       <c r="I48" s="17"/>
       <c r="J48" s="17"/>
@@ -2631,11 +2687,11 @@
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
       <c r="H49" s="17"/>
       <c r="I49" s="17"/>
       <c r="J49" s="17"/>
@@ -2653,11 +2709,11 @@
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
       <c r="H50" s="17"/>
       <c r="I50" s="17"/>
       <c r="J50" s="17"/>
@@ -2675,11 +2731,11 @@
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="17"/>
       <c r="B51" s="17"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
       <c r="H51" s="17"/>
       <c r="I51" s="17"/>
       <c r="J51" s="17"/>
@@ -2701,19 +2757,19 @@
       <c r="B52" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="18" t="s">
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="19" t="s">
         <v>37</v>
       </c>
       <c r="I52" s="17"/>
       <c r="J52" s="17"/>
-      <c r="K52" s="18" t="s">
+      <c r="K52" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L52" s="17"/>
@@ -2733,11 +2789,11 @@
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="17"/>
       <c r="B53" s="17"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
       <c r="H53" s="17"/>
       <c r="I53" s="17"/>
       <c r="J53" s="17"/>
@@ -2755,11 +2811,11 @@
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
       <c r="H54" s="17"/>
       <c r="I54" s="17"/>
       <c r="J54" s="17"/>
@@ -2777,11 +2833,11 @@
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
       <c r="H55" s="17"/>
       <c r="I55" s="17"/>
       <c r="J55" s="17"/>
@@ -2799,11 +2855,11 @@
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
       <c r="H56" s="17"/>
       <c r="I56" s="17"/>
       <c r="J56" s="17"/>
@@ -2821,11 +2877,11 @@
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
       <c r="H57" s="17"/>
       <c r="I57" s="17"/>
       <c r="J57" s="17"/>
@@ -2843,11 +2899,11 @@
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="17"/>
       <c r="B58" s="17"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
       <c r="H58" s="17"/>
       <c r="I58" s="17"/>
       <c r="J58" s="17"/>
@@ -2865,11 +2921,11 @@
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
       <c r="H59" s="17"/>
       <c r="I59" s="17"/>
       <c r="J59" s="17"/>
@@ -2887,11 +2943,11 @@
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="17"/>
       <c r="B60" s="17"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
       <c r="H60" s="17"/>
       <c r="I60" s="17"/>
       <c r="J60" s="17"/>
@@ -2909,11 +2965,11 @@
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
       <c r="J61" s="17"/>
@@ -2931,11 +2987,11 @@
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="17"/>
       <c r="B62" s="17"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
       <c r="J62" s="17"/>
@@ -2953,11 +3009,11 @@
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
       <c r="H63" s="17"/>
       <c r="I63" s="17"/>
       <c r="J63" s="17"/>
@@ -2975,11 +3031,11 @@
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
       <c r="H64" s="17"/>
       <c r="I64" s="17"/>
       <c r="J64" s="17"/>
@@ -3001,19 +3057,19 @@
       <c r="B65" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="18" t="s">
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="19" t="s">
         <v>39</v>
       </c>
       <c r="I65" s="17"/>
       <c r="J65" s="17"/>
-      <c r="K65" s="18" t="s">
+      <c r="K65" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L65" s="17"/>
@@ -3033,11 +3089,11 @@
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
       <c r="H66" s="17"/>
       <c r="I66" s="17"/>
       <c r="J66" s="17"/>
@@ -3055,11 +3111,11 @@
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="17"/>
       <c r="B67" s="17"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
       <c r="H67" s="17"/>
       <c r="I67" s="17"/>
       <c r="J67" s="17"/>
@@ -3077,11 +3133,11 @@
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="17"/>
       <c r="B68" s="17"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
       <c r="J68" s="17"/>
@@ -3099,11 +3155,11 @@
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
-      <c r="C69" s="16"/>
-      <c r="D69" s="16"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="16"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
       <c r="H69" s="17"/>
       <c r="I69" s="17"/>
       <c r="J69" s="17"/>
@@ -3121,11 +3177,11 @@
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="17"/>
       <c r="B70" s="17"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="16"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
       <c r="H70" s="17"/>
       <c r="I70" s="17"/>
       <c r="J70" s="17"/>
@@ -3143,11 +3199,11 @@
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="16"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
       <c r="H71" s="17"/>
       <c r="I71" s="17"/>
       <c r="J71" s="17"/>
@@ -3165,11 +3221,11 @@
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="17"/>
       <c r="B72" s="17"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="16"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
       <c r="J72" s="17"/>
@@ -3187,11 +3243,11 @@
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="17"/>
       <c r="B73" s="17"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="16"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
       <c r="J73" s="17"/>
@@ -3209,11 +3265,11 @@
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
       <c r="H74" s="17"/>
       <c r="I74" s="17"/>
       <c r="J74" s="17"/>
@@ -3231,11 +3287,11 @@
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="17"/>
       <c r="B75" s="17"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="16"/>
-      <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
-      <c r="G75" s="16"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
       <c r="H75" s="17"/>
       <c r="I75" s="17"/>
       <c r="J75" s="17"/>
@@ -3253,11 +3309,11 @@
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="16"/>
-      <c r="E76" s="16"/>
-      <c r="F76" s="16"/>
-      <c r="G76" s="16"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
       <c r="H76" s="17"/>
       <c r="I76" s="17"/>
       <c r="J76" s="17"/>
@@ -3275,11 +3331,11 @@
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="17"/>
       <c r="B77" s="17"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="16"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="16"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
       <c r="H77" s="17"/>
       <c r="I77" s="17"/>
       <c r="J77" s="17"/>
@@ -3301,19 +3357,19 @@
       <c r="B78" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C78" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="16"/>
-      <c r="H78" s="18" t="s">
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="19" t="s">
         <v>40</v>
       </c>
       <c r="I78" s="17"/>
       <c r="J78" s="17"/>
-      <c r="K78" s="18" t="s">
+      <c r="K78" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L78" s="17"/>
@@ -3333,11 +3389,11 @@
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="17"/>
       <c r="B79" s="17"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="16"/>
-      <c r="E79" s="16"/>
-      <c r="F79" s="16"/>
-      <c r="G79" s="16"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
       <c r="H79" s="17"/>
       <c r="I79" s="17"/>
       <c r="J79" s="17"/>
@@ -3355,11 +3411,11 @@
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="17"/>
       <c r="B80" s="17"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-      <c r="E80" s="16"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="16"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
       <c r="J80" s="17"/>
@@ -3377,11 +3433,11 @@
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="17"/>
       <c r="B81" s="17"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="16"/>
-      <c r="E81" s="16"/>
-      <c r="F81" s="16"/>
-      <c r="G81" s="16"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
       <c r="J81" s="17"/>
@@ -3399,11 +3455,11 @@
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="17"/>
       <c r="B82" s="17"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="16"/>
-      <c r="E82" s="16"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="16"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
       <c r="J82" s="17"/>
@@ -3421,11 +3477,11 @@
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="17"/>
       <c r="B83" s="17"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
-      <c r="G83" s="16"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
       <c r="J83" s="17"/>
@@ -3443,11 +3499,11 @@
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="17"/>
       <c r="B84" s="17"/>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="16"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
       <c r="J84" s="17"/>
@@ -3465,11 +3521,11 @@
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="17"/>
       <c r="B85" s="17"/>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16"/>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="16"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
       <c r="J85" s="17"/>
@@ -3487,11 +3543,11 @@
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="17"/>
       <c r="B86" s="17"/>
-      <c r="C86" s="16"/>
-      <c r="D86" s="16"/>
-      <c r="E86" s="16"/>
-      <c r="F86" s="16"/>
-      <c r="G86" s="16"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
       <c r="J86" s="17"/>
@@ -3509,11 +3565,11 @@
     <row r="87" spans="1:20" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="17"/>
       <c r="B87" s="17"/>
-      <c r="C87" s="16"/>
-      <c r="D87" s="16"/>
-      <c r="E87" s="16"/>
-      <c r="F87" s="16"/>
-      <c r="G87" s="16"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
       <c r="J87" s="17"/>
@@ -3531,11 +3587,11 @@
     <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="17"/>
       <c r="B88" s="17"/>
-      <c r="C88" s="16"/>
-      <c r="D88" s="16"/>
-      <c r="E88" s="16"/>
-      <c r="F88" s="16"/>
-      <c r="G88" s="16"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="18"/>
       <c r="H88" s="17"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -3553,11 +3609,11 @@
     <row r="89" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="17"/>
       <c r="B89" s="17"/>
-      <c r="C89" s="16"/>
-      <c r="D89" s="16"/>
-      <c r="E89" s="16"/>
-      <c r="F89" s="16"/>
-      <c r="G89" s="16"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
       <c r="H89" s="17"/>
       <c r="I89" s="17"/>
       <c r="J89" s="17"/>
@@ -3575,11 +3631,11 @@
     <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="17"/>
       <c r="B90" s="17"/>
-      <c r="C90" s="16"/>
-      <c r="D90" s="16"/>
-      <c r="E90" s="16"/>
-      <c r="F90" s="16"/>
-      <c r="G90" s="16"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
       <c r="J90" s="17"/>
@@ -3601,19 +3657,19 @@
       <c r="B91" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C91" s="16" t="s">
+      <c r="C91" s="18" t="s">
         <v>93</v>
       </c>
       <c r="D91" s="17"/>
       <c r="E91" s="17"/>
       <c r="F91" s="17"/>
       <c r="G91" s="17"/>
-      <c r="H91" s="18" t="s">
+      <c r="H91" s="19" t="s">
         <v>55</v>
       </c>
       <c r="I91" s="17"/>
       <c r="J91" s="17"/>
-      <c r="K91" s="18" t="s">
+      <c r="K91" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L91" s="17"/>
@@ -3637,19 +3693,19 @@
       <c r="B92" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C92" s="16" t="s">
+      <c r="C92" s="18" t="s">
         <v>94</v>
       </c>
       <c r="D92" s="17"/>
       <c r="E92" s="17"/>
       <c r="F92" s="17"/>
       <c r="G92" s="17"/>
-      <c r="H92" s="18" t="s">
+      <c r="H92" s="19" t="s">
         <v>61</v>
       </c>
       <c r="I92" s="17"/>
       <c r="J92" s="17"/>
-      <c r="K92" s="18" t="s">
+      <c r="K92" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L92" s="17"/>
@@ -3673,19 +3729,19 @@
       <c r="B93" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C93" s="16" t="s">
+      <c r="C93" s="18" t="s">
         <v>95</v>
       </c>
       <c r="D93" s="17"/>
       <c r="E93" s="17"/>
       <c r="F93" s="17"/>
       <c r="G93" s="17"/>
-      <c r="H93" s="18" t="s">
+      <c r="H93" s="19" t="s">
         <v>59</v>
       </c>
       <c r="I93" s="17"/>
       <c r="J93" s="17"/>
-      <c r="K93" s="18" t="s">
+      <c r="K93" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L93" s="17"/>
@@ -3709,24 +3765,24 @@
       <c r="B94" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C94" s="16" t="s">
+      <c r="C94" s="18" t="s">
         <v>116</v>
       </c>
       <c r="D94" s="17"/>
       <c r="E94" s="17"/>
       <c r="F94" s="17"/>
       <c r="G94" s="17"/>
-      <c r="H94" s="18" t="s">
+      <c r="H94" s="19" t="s">
         <v>117</v>
       </c>
       <c r="I94" s="17"/>
       <c r="J94" s="17"/>
-      <c r="K94" s="18" t="s">
+      <c r="K94" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L94" s="17"/>
       <c r="M94" s="17"/>
-      <c r="N94" s="18" t="s">
+      <c r="N94" s="19" t="s">
         <v>118</v>
       </c>
       <c r="O94" s="17"/>
@@ -3745,19 +3801,19 @@
       <c r="B95" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C95" s="16" t="s">
+      <c r="C95" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D95" s="16"/>
-      <c r="E95" s="16"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="16"/>
-      <c r="H95" s="18" t="s">
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="19" t="s">
         <v>125</v>
       </c>
       <c r="I95" s="17"/>
       <c r="J95" s="17"/>
-      <c r="K95" s="18" t="s">
+      <c r="K95" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L95" s="17"/>
@@ -3777,11 +3833,11 @@
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="17"/>
       <c r="B96" s="17"/>
-      <c r="C96" s="16"/>
-      <c r="D96" s="16"/>
-      <c r="E96" s="16"/>
-      <c r="F96" s="16"/>
-      <c r="G96" s="16"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
       <c r="H96" s="17"/>
       <c r="I96" s="17"/>
       <c r="J96" s="17"/>
@@ -3799,11 +3855,11 @@
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="17"/>
       <c r="B97" s="17"/>
-      <c r="C97" s="16"/>
-      <c r="D97" s="16"/>
-      <c r="E97" s="16"/>
-      <c r="F97" s="16"/>
-      <c r="G97" s="16"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
       <c r="J97" s="17"/>
@@ -3821,11 +3877,11 @@
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="17"/>
       <c r="B98" s="17"/>
-      <c r="C98" s="16"/>
-      <c r="D98" s="16"/>
-      <c r="E98" s="16"/>
-      <c r="F98" s="16"/>
-      <c r="G98" s="16"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
       <c r="H98" s="17"/>
       <c r="I98" s="17"/>
       <c r="J98" s="17"/>
@@ -3843,11 +3899,11 @@
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="17"/>
       <c r="B99" s="17"/>
-      <c r="C99" s="16"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="16"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="18"/>
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
       <c r="J99" s="17"/>
@@ -3865,11 +3921,11 @@
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
-      <c r="C100" s="16"/>
-      <c r="D100" s="16"/>
-      <c r="E100" s="16"/>
-      <c r="F100" s="16"/>
-      <c r="G100" s="16"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
       <c r="J100" s="17"/>
@@ -3887,11 +3943,11 @@
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="17"/>
       <c r="B101" s="17"/>
-      <c r="C101" s="16"/>
-      <c r="D101" s="16"/>
-      <c r="E101" s="16"/>
-      <c r="F101" s="16"/>
-      <c r="G101" s="16"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
       <c r="H101" s="17"/>
       <c r="I101" s="17"/>
       <c r="J101" s="17"/>
@@ -3909,11 +3965,11 @@
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="17"/>
       <c r="B102" s="17"/>
-      <c r="C102" s="16"/>
-      <c r="D102" s="16"/>
-      <c r="E102" s="16"/>
-      <c r="F102" s="16"/>
-      <c r="G102" s="16"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
       <c r="J102" s="17"/>
@@ -3931,11 +3987,11 @@
     <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="17"/>
       <c r="B103" s="17"/>
-      <c r="C103" s="16"/>
-      <c r="D103" s="16"/>
-      <c r="E103" s="16"/>
-      <c r="F103" s="16"/>
-      <c r="G103" s="16"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
       <c r="H103" s="17"/>
       <c r="I103" s="17"/>
       <c r="J103" s="17"/>
@@ -3953,11 +4009,11 @@
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="17"/>
       <c r="B104" s="17"/>
-      <c r="C104" s="16"/>
-      <c r="D104" s="16"/>
-      <c r="E104" s="16"/>
-      <c r="F104" s="16"/>
-      <c r="G104" s="16"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
       <c r="H104" s="17"/>
       <c r="I104" s="17"/>
       <c r="J104" s="17"/>
@@ -3975,11 +4031,11 @@
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="17"/>
       <c r="B105" s="17"/>
-      <c r="C105" s="16"/>
-      <c r="D105" s="16"/>
-      <c r="E105" s="16"/>
-      <c r="F105" s="16"/>
-      <c r="G105" s="16"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
       <c r="H105" s="17"/>
       <c r="I105" s="17"/>
       <c r="J105" s="17"/>
@@ -3997,11 +4053,11 @@
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="17"/>
       <c r="B106" s="17"/>
-      <c r="C106" s="16"/>
-      <c r="D106" s="16"/>
-      <c r="E106" s="16"/>
-      <c r="F106" s="16"/>
-      <c r="G106" s="16"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
       <c r="H106" s="17"/>
       <c r="I106" s="17"/>
       <c r="J106" s="17"/>
@@ -4019,11 +4075,11 @@
     <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="17"/>
       <c r="B107" s="17"/>
-      <c r="C107" s="16"/>
-      <c r="D107" s="16"/>
-      <c r="E107" s="16"/>
-      <c r="F107" s="16"/>
-      <c r="G107" s="16"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18"/>
+      <c r="F107" s="18"/>
+      <c r="G107" s="18"/>
       <c r="H107" s="17"/>
       <c r="I107" s="17"/>
       <c r="J107" s="17"/>
@@ -4040,61 +4096,23 @@
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="A95:A107"/>
-    <mergeCell ref="B95:B107"/>
-    <mergeCell ref="C95:G107"/>
-    <mergeCell ref="H95:J107"/>
-    <mergeCell ref="K95:M107"/>
-    <mergeCell ref="N93:S93"/>
-    <mergeCell ref="B78:B90"/>
-    <mergeCell ref="C78:G90"/>
-    <mergeCell ref="H78:J90"/>
-    <mergeCell ref="K78:M90"/>
-    <mergeCell ref="N78:S90"/>
-    <mergeCell ref="K91:M91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="N92:S92"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="H91:J91"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="H15:J26"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="N95:S107"/>
-    <mergeCell ref="T95:T107"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:R13"/>
-    <mergeCell ref="T65:T77"/>
-    <mergeCell ref="T52:T64"/>
-    <mergeCell ref="N52:S64"/>
-    <mergeCell ref="T78:T90"/>
-    <mergeCell ref="T15:T26"/>
-    <mergeCell ref="N27:S39"/>
-    <mergeCell ref="T27:T39"/>
-    <mergeCell ref="N40:S51"/>
-    <mergeCell ref="T40:T51"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="A78:A90"/>
-    <mergeCell ref="K40:M51"/>
-    <mergeCell ref="A40:A51"/>
-    <mergeCell ref="B40:B51"/>
-    <mergeCell ref="C40:G51"/>
-    <mergeCell ref="H52:J64"/>
-    <mergeCell ref="K52:M64"/>
-    <mergeCell ref="C52:G64"/>
-    <mergeCell ref="H40:J51"/>
-    <mergeCell ref="A65:A77"/>
-    <mergeCell ref="B65:B77"/>
-    <mergeCell ref="C65:G77"/>
-    <mergeCell ref="H65:J77"/>
-    <mergeCell ref="K65:M77"/>
-    <mergeCell ref="A52:A64"/>
-    <mergeCell ref="B52:B64"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="N65:S77"/>
+    <mergeCell ref="N91:S91"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="H27:J39"/>
     <mergeCell ref="K27:M39"/>
@@ -4119,30 +4137,68 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:R4"/>
     <mergeCell ref="A15:A26"/>
+    <mergeCell ref="A40:A51"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="C40:G51"/>
+    <mergeCell ref="H52:J64"/>
+    <mergeCell ref="K52:M64"/>
+    <mergeCell ref="C52:G64"/>
+    <mergeCell ref="H40:J51"/>
+    <mergeCell ref="A65:A77"/>
+    <mergeCell ref="B65:B77"/>
+    <mergeCell ref="C65:G77"/>
+    <mergeCell ref="H65:J77"/>
+    <mergeCell ref="K65:M77"/>
+    <mergeCell ref="A52:A64"/>
+    <mergeCell ref="B52:B64"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="H15:J26"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="N95:S107"/>
+    <mergeCell ref="T95:T107"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:R13"/>
+    <mergeCell ref="T65:T77"/>
+    <mergeCell ref="T52:T64"/>
+    <mergeCell ref="N52:S64"/>
+    <mergeCell ref="T78:T90"/>
+    <mergeCell ref="T15:T26"/>
+    <mergeCell ref="N27:S39"/>
+    <mergeCell ref="T27:T39"/>
+    <mergeCell ref="N40:S51"/>
+    <mergeCell ref="T40:T51"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K40:M51"/>
     <mergeCell ref="C94:G94"/>
     <mergeCell ref="H94:J94"/>
+    <mergeCell ref="A95:A107"/>
+    <mergeCell ref="B95:B107"/>
+    <mergeCell ref="C95:G107"/>
+    <mergeCell ref="H95:J107"/>
+    <mergeCell ref="K95:M107"/>
+    <mergeCell ref="N93:S93"/>
+    <mergeCell ref="B78:B90"/>
+    <mergeCell ref="C78:G90"/>
+    <mergeCell ref="H78:J90"/>
+    <mergeCell ref="K78:M90"/>
+    <mergeCell ref="N78:S90"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="N92:S92"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="A78:A90"/>
     <mergeCell ref="K94:M94"/>
     <mergeCell ref="N94:S94"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C11:G11"/>
     <mergeCell ref="C93:G93"/>
     <mergeCell ref="H93:J93"/>
     <mergeCell ref="K93:M93"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="N65:S77"/>
-    <mergeCell ref="N91:S91"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="K9:R9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4193,15 +4249,15 @@
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -4216,26 +4272,26 @@
       <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -4245,29 +4301,29 @@
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20" t="s">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
       <c r="T3" s="6" t="s">
         <v>18</v>
       </c>
@@ -4279,29 +4335,29 @@
       <c r="B4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="17" t="s">
         <v>121</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
       <c r="T4" s="12" t="s">
         <v>51</v>
       </c>
@@ -4336,18 +4392,18 @@
       <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="18" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="17" t="s">
         <v>4</v>
       </c>
@@ -4372,14 +4428,14 @@
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="18" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="19" t="s">
         <v>53</v>
       </c>
       <c r="I7" s="17"/>
@@ -4403,14 +4459,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="N7:S7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:S6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="K7:M7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="C3:G3"/>
@@ -4420,6 +4468,14 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:S4"/>
     <mergeCell ref="K3:S3"/>
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:S6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="K7:M7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4432,10 +4488,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S20"/>
+  <dimension ref="A2:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="F20" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21:R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4454,18 +4510,18 @@
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="18" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="17" t="s">
         <v>14</v>
       </c>
@@ -4487,18 +4543,18 @@
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="21" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
       <c r="K4" s="17" t="s">
         <v>19</v>
       </c>
@@ -4520,18 +4576,18 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="21" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
       <c r="K6" s="17" t="s">
         <v>15</v>
       </c>
@@ -4553,18 +4609,18 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="18" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
       <c r="K8" s="17" t="s">
         <v>21</v>
       </c>
@@ -4586,18 +4642,18 @@
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="18" t="s">
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
       <c r="K10" s="17" t="s">
         <v>44</v>
       </c>
@@ -4619,18 +4675,18 @@
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="18" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="17" t="s">
         <v>46</v>
       </c>
@@ -4652,18 +4708,18 @@
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="18" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
       <c r="K14" s="17" t="s">
         <v>13</v>
       </c>
@@ -4685,18 +4741,18 @@
       <c r="B16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="18" t="s">
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
       <c r="K16" s="17" t="s">
         <v>137</v>
       </c>
@@ -4718,18 +4774,18 @@
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="21" t="s">
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
       <c r="K17" s="17" t="s">
         <v>17</v>
       </c>
@@ -4751,18 +4807,18 @@
       <c r="B18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="21" t="s">
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
       <c r="K18" s="17" t="s">
         <v>136</v>
       </c>
@@ -4784,18 +4840,18 @@
       <c r="B19" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="21" t="s">
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
       <c r="K19" s="17" t="s">
         <v>143</v>
       </c>
@@ -4817,18 +4873,18 @@
       <c r="B20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="21" t="s">
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
       <c r="K20" s="17" t="s">
         <v>148</v>
       </c>
@@ -4843,14 +4899,58 @@
         <v>36</v>
       </c>
     </row>
+    <row r="21" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:R20"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:R19"/>
+  <mergeCells count="39">
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:R16"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="K18:R18"/>
@@ -4860,12 +4960,6 @@
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="K10:R10"/>
     <mergeCell ref="C12:G12"/>
@@ -4873,14 +4967,12 @@
     <mergeCell ref="K12:R12"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:R14"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:R17"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:R16"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:R20"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:R19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -4895,8 +4987,9 @@
     <hyperlink ref="C16" r:id="rId10"/>
     <hyperlink ref="C19" r:id="rId11"/>
     <hyperlink ref="C20" r:id="rId12"/>
+    <hyperlink ref="C21" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego HATEOAS a todos los casos de los servicios en admin
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15195" windowHeight="4170" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15195" windowHeight="4170"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="178">
   <si>
     <t>Recurso</t>
   </si>
@@ -183,11 +183,6 @@
   </si>
   <si>
     <t>Devuelve una parada especifica indicada en la url.</t>
-  </si>
-  <si>
-    <t>{
-"Encontrado": true
-}</t>
   </si>
   <si>
     <t>Mediante una placa enviada modifica el estado del bus que coincide con dicha placa.</t>
@@ -539,9 +534,6 @@
     <t>itinerario/eliminar/{$clave}</t>
   </si>
   <si>
-    <t>http://localhost:8080/cloudBRT/api/admin/itinerario/eliminar/I3T3</t>
-  </si>
-  <si>
     <t>Encuentra y si existe elimina el itinerario con la clave especificada de lo contrario no se efectua la tarea.</t>
   </si>
   <si>
@@ -774,18 +766,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>{
-  "Creado": true,
-  "Recurso": "http://localhost:8080/cloudBRT/api/monitoreo/buses/TET456"
-}</t>
-  </si>
-  <si>
-    <t>{
-  "Modificado": true,
-  "Recurso": "http://localhost:8080/cloudBRT/api/monitoreo/buses/AMB123"
-}</t>
-  </si>
-  <si>
     <t>paradas/{$parada}</t>
   </si>
   <si>
@@ -793,12 +773,6 @@
   </si>
   <si>
     <t>paradas/</t>
-  </si>
-  <si>
-    <t>{
-  "Creado": true,
-  "Recurso": "http://localhost:8080/cloudBRT/api/monitoreo/paradas/ST19"
-}</t>
   </si>
   <si>
     <t>{
@@ -814,12 +788,6 @@
     <t>http://localhost:8080/cloudBRT/api/admin/paradas</t>
   </si>
   <si>
-    <t>{
-  "ParadasEliminadas": true,
-  "Recurso": "http://localhost:8080/cloudBRT/api/monitoreo/rutas/P8"
-}</t>
-  </si>
-  <si>
     <t>http://localhost:8080/cloudBRT/api/admin/rutas/P8/paradas</t>
   </si>
   <si>
@@ -827,12 +795,6 @@
   </si>
   <si>
     <t>http://localhost:8080/cloudBRT/api/admin/rutas/P2/paradas/2</t>
-  </si>
-  <si>
-    <t>{
-  "ParadaEliminada": true,
-  "Recurso": "http://localhost:8080/cloudBRT/api/monitoreo/rutas/P2"
-}</t>
   </si>
   <si>
     <t>/rutas/{nombreRuta}/paradas/{posicion}</t>
@@ -851,21 +813,10 @@
 }</t>
   </si>
   <si>
-    <t>{
-  "Elimino": true
-}</t>
-  </si>
-  <si>
     <t>http://localhost:8080/cloudBRT/api/admin/rutas/P8</t>
   </si>
   <si>
     <t>/rutas/{nombreRuta}</t>
-  </si>
-  <si>
-    <t>{
-  "Encontrado": true,
-  "Recurso": "http://localhost:8080/cloudBRT/api/monitoreo/rutas/P8"
-}</t>
   </si>
   <si>
     <t>http://localhost:8080/cloudBRT/api/admin/rutas</t>
@@ -971,12 +922,6 @@
   </si>
   <si>
     <t>http://localhost:8080/cloudBRT/api/admin/conductores/1098755547</t>
-  </si>
-  <si>
-    <t>{
-  "Creado": true,
-  "RecursoConductor": "No implementado su servicio de consulta aun"
-}</t>
   </si>
   <si>
     <t>{
@@ -997,12 +942,6 @@
   </si>
   <si>
     <t>/conductores/{Dato}</t>
-  </si>
-  <si>
-    <t>{
-  "Modificado": true,
-  "RecursoConductor": "No implementado su servicio de consulta aun"
-}</t>
   </si>
   <si>
     <t>{
@@ -1154,6 +1093,81 @@
   </si>
   <si>
     <t>Devuelve un conductor especifico dado en la url</t>
+  </si>
+  <si>
+    <t>{
+"Eliminado":true,
+"RecursoBus": "http://localhost:8080/cloudBRT/api/monitoreo/buses"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "Modificado": true,
+  "RecursoBus": "http://localhost:8080/cloudBRT/api/monitoreo/buses/AMB123"
+}</t>
+  </si>
+  <si>
+    <t>{
+"Eliminado":true,
+"RecursoRuta": "http://localhost:8080/cloudBRT/api/monitoreo/paradas"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "ParadasEliminadas": true,
+  "RecursoRuta": "http://localhost:8080/cloudBRT/api/monitoreo/rutas/P8"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "ParadaEliminada": true,
+  "RecursoRuta": "http://localhost:8080/cloudBRT/api/monitoreo/rutas/P2"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "Creado": true,
+  "RecursoBus": "http://localhost:8080/cloudBRT/api/monitoreo/buses/TET456"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "Creado": true,
+  "RecursoParada": "http://localhost:8080/cloudBRT/api/monitoreo/paradas/ST19"
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/admin/itinerario/I3T3</t>
+  </si>
+  <si>
+    <t>{
+"Eliminado":true,
+"RecursoItinerario": "http://localhost:8080/cloudBRT/api/monitoreo/itinerarios"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "Creado": true,
+  "RecursoRuta": "http://localhost:8080/cloudBRT/api/monitoreo/rutas/P8"
+}</t>
+  </si>
+  <si>
+    <t>{
+"Eliminado":true,
+"RecursoRecorrido": "http://localhost:8080/cloudBRT/api/monitoreo/recorridos"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "Creado": true,
+  "RecursoConductor": "http://localhost:8080/cloudBRT/api/monitoreo/conductores/1098747294"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "Modificado": true,
+  "RecursoConductor": "http://localhost:8080/cloudBRT/api/monitoreo/conductores/1098747294"
+}</t>
   </si>
 </sst>
 </file>
@@ -1607,8 +1621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T108"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView tabSelected="1" topLeftCell="F45" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K94" sqref="K94:M94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,25 +1720,25 @@
     </row>
     <row r="4" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="22" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
@@ -1734,30 +1748,30 @@
       <c r="Q4" s="21"/>
       <c r="R4" s="21"/>
       <c r="S4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>79</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>81</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="22" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
       <c r="K5" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
@@ -1767,30 +1781,30 @@
       <c r="Q5" s="21"/>
       <c r="R5" s="21"/>
       <c r="S5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
@@ -1800,30 +1814,30 @@
       <c r="Q6" s="21"/>
       <c r="R6" s="21"/>
       <c r="S6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="22" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
       <c r="K7" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
@@ -1833,30 +1847,30 @@
       <c r="Q7" s="21"/>
       <c r="R7" s="21"/>
       <c r="S7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="22" t="s">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
       <c r="K8" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
@@ -1866,30 +1880,30 @@
       <c r="Q8" s="21"/>
       <c r="R8" s="21"/>
       <c r="S8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="22" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
@@ -1899,30 +1913,30 @@
       <c r="Q9" s="21"/>
       <c r="R9" s="21"/>
       <c r="S9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="22" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
@@ -1932,30 +1946,30 @@
       <c r="Q10" s="21"/>
       <c r="R10" s="21"/>
       <c r="S10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="22" t="s">
-        <v>108</v>
+        <v>174</v>
       </c>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
@@ -1965,30 +1979,30 @@
       <c r="Q11" s="21"/>
       <c r="R11" s="21"/>
       <c r="S11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>62</v>
+        <v>172</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="22" t="s">
-        <v>22</v>
+        <v>173</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
@@ -1998,30 +2012,30 @@
       <c r="Q12" s="21"/>
       <c r="R12" s="21"/>
       <c r="S12" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="22" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
@@ -2031,7 +2045,7 @@
       <c r="Q13" s="21"/>
       <c r="R13" s="21"/>
       <c r="S13" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2066,30 +2080,30 @@
     </row>
     <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>87</v>
-      </c>
       <c r="C15" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
       <c r="K15" s="22" t="s">
-        <v>88</v>
+        <v>170</v>
       </c>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O15" s="21"/>
       <c r="P15" s="21"/>
@@ -2097,7 +2111,7 @@
       <c r="R15" s="21"/>
       <c r="S15" s="21"/>
       <c r="T15" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2344,30 +2358,30 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="22" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
       <c r="K27" s="22" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
       <c r="N27" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O27" s="21"/>
       <c r="P27" s="21"/>
@@ -2375,7 +2389,7 @@
       <c r="R27" s="21"/>
       <c r="S27" s="21"/>
       <c r="T27" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -2644,13 +2658,13 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
@@ -2660,12 +2674,12 @@
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
       <c r="K40" s="22" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
       <c r="N40" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O40" s="21"/>
       <c r="P40" s="21"/>
@@ -2673,7 +2687,7 @@
       <c r="R40" s="21"/>
       <c r="S40" s="21"/>
       <c r="T40" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -2920,13 +2934,13 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
@@ -2936,12 +2950,12 @@
       <c r="I52" s="21"/>
       <c r="J52" s="21"/>
       <c r="K52" s="22" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="L52" s="21"/>
       <c r="M52" s="21"/>
       <c r="N52" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O52" s="21"/>
       <c r="P52" s="21"/>
@@ -2949,7 +2963,7 @@
       <c r="R52" s="21"/>
       <c r="S52" s="21"/>
       <c r="T52" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
@@ -3218,30 +3232,30 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
       <c r="G65" s="20"/>
       <c r="H65" s="22" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="I65" s="21"/>
       <c r="J65" s="21"/>
       <c r="K65" s="22" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="L65" s="21"/>
       <c r="M65" s="21"/>
       <c r="N65" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O65" s="21"/>
       <c r="P65" s="21"/>
@@ -3249,7 +3263,7 @@
       <c r="R65" s="21"/>
       <c r="S65" s="21"/>
       <c r="T65" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
@@ -3518,30 +3532,30 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D78" s="20"/>
       <c r="E78" s="20"/>
       <c r="F78" s="20"/>
       <c r="G78" s="20"/>
       <c r="H78" s="22" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="I78" s="21"/>
       <c r="J78" s="21"/>
       <c r="K78" s="22" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="L78" s="21"/>
       <c r="M78" s="21"/>
       <c r="N78" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O78" s="21"/>
       <c r="P78" s="21"/>
@@ -3549,7 +3563,7 @@
       <c r="R78" s="21"/>
       <c r="S78" s="21"/>
       <c r="T78" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
@@ -3818,30 +3832,30 @@
     </row>
     <row r="91" spans="1:20" s="5" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
       <c r="F91" s="21"/>
       <c r="G91" s="21"/>
       <c r="H91" s="22" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I91" s="21"/>
       <c r="J91" s="21"/>
       <c r="K91" s="22" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="L91" s="21"/>
       <c r="M91" s="21"/>
       <c r="N91" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O91" s="21"/>
       <c r="P91" s="21"/>
@@ -3849,35 +3863,35 @@
       <c r="R91" s="21"/>
       <c r="S91" s="21"/>
       <c r="T91" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="92" spans="1:20" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
       <c r="F92" s="21"/>
       <c r="G92" s="21"/>
       <c r="H92" s="22" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="I92" s="21"/>
       <c r="J92" s="21"/>
       <c r="K92" s="22" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="L92" s="21"/>
       <c r="M92" s="21"/>
       <c r="N92" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O92" s="21"/>
       <c r="P92" s="21"/>
@@ -3885,35 +3899,35 @@
       <c r="R92" s="21"/>
       <c r="S92" s="21"/>
       <c r="T92" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="93" spans="1:20" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
       <c r="F93" s="21"/>
       <c r="G93" s="21"/>
       <c r="H93" s="22" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="I93" s="21"/>
       <c r="J93" s="21"/>
       <c r="K93" s="22" t="s">
-        <v>133</v>
+        <v>176</v>
       </c>
       <c r="L93" s="21"/>
       <c r="M93" s="21"/>
       <c r="N93" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O93" s="21"/>
       <c r="P93" s="21"/>
@@ -3921,35 +3935,35 @@
       <c r="R93" s="21"/>
       <c r="S93" s="21"/>
       <c r="T93" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="94" spans="1:20" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
       <c r="F94" s="21"/>
       <c r="G94" s="21"/>
       <c r="H94" s="22" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="I94" s="21"/>
       <c r="J94" s="21"/>
       <c r="K94" s="22" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="L94" s="21"/>
       <c r="M94" s="21"/>
       <c r="N94" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O94" s="21"/>
       <c r="P94" s="21"/>
@@ -3957,35 +3971,35 @@
       <c r="R94" s="21"/>
       <c r="S94" s="21"/>
       <c r="T94" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D95" s="20"/>
       <c r="E95" s="20"/>
       <c r="F95" s="20"/>
       <c r="G95" s="20"/>
       <c r="H95" s="22" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="I95" s="21"/>
       <c r="J95" s="21"/>
       <c r="K95" s="22" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="L95" s="21"/>
       <c r="M95" s="21"/>
       <c r="N95" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O95" s="21"/>
       <c r="P95" s="21"/>
@@ -3993,7 +4007,7 @@
       <c r="R95" s="21"/>
       <c r="S95" s="21"/>
       <c r="T95" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
@@ -4262,13 +4276,13 @@
     </row>
     <row r="108" spans="1:20" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B108" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -4278,12 +4292,12 @@
       <c r="I108" s="21"/>
       <c r="J108" s="21"/>
       <c r="K108" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L108" s="21"/>
       <c r="M108" s="21"/>
       <c r="N108" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O108" s="21"/>
       <c r="P108" s="21"/>
@@ -4291,33 +4305,72 @@
       <c r="R108" s="21"/>
       <c r="S108" s="21"/>
       <c r="T108" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:J108"/>
-    <mergeCell ref="K108:M108"/>
-    <mergeCell ref="N108:S108"/>
-    <mergeCell ref="A95:A107"/>
-    <mergeCell ref="B95:B107"/>
-    <mergeCell ref="C95:G107"/>
-    <mergeCell ref="H95:J107"/>
-    <mergeCell ref="K95:M107"/>
-    <mergeCell ref="N93:S93"/>
-    <mergeCell ref="B78:B90"/>
-    <mergeCell ref="C78:G90"/>
-    <mergeCell ref="H78:J90"/>
-    <mergeCell ref="K78:M90"/>
-    <mergeCell ref="N78:S90"/>
-    <mergeCell ref="K91:M91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="N92:S92"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="N65:S77"/>
+    <mergeCell ref="N91:S91"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="H15:J26"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="H27:J39"/>
+    <mergeCell ref="K27:M39"/>
+    <mergeCell ref="C27:G39"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A27:A39"/>
+    <mergeCell ref="B27:B39"/>
+    <mergeCell ref="N14:S14"/>
+    <mergeCell ref="N15:S26"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M26"/>
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="C15:G26"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="C40:G51"/>
+    <mergeCell ref="H52:J64"/>
+    <mergeCell ref="K52:M64"/>
+    <mergeCell ref="C52:G64"/>
+    <mergeCell ref="H40:J51"/>
+    <mergeCell ref="A65:A77"/>
+    <mergeCell ref="B65:B77"/>
+    <mergeCell ref="C65:G77"/>
+    <mergeCell ref="H65:J77"/>
+    <mergeCell ref="K65:M77"/>
+    <mergeCell ref="A52:A64"/>
+    <mergeCell ref="B52:B64"/>
     <mergeCell ref="A78:A90"/>
     <mergeCell ref="K94:M94"/>
     <mergeCell ref="N94:S94"/>
@@ -4342,67 +4395,28 @@
     <mergeCell ref="C94:G94"/>
     <mergeCell ref="H94:J94"/>
     <mergeCell ref="A40:A51"/>
-    <mergeCell ref="B40:B51"/>
-    <mergeCell ref="C40:G51"/>
-    <mergeCell ref="H52:J64"/>
-    <mergeCell ref="K52:M64"/>
-    <mergeCell ref="C52:G64"/>
-    <mergeCell ref="H40:J51"/>
-    <mergeCell ref="A65:A77"/>
-    <mergeCell ref="B65:B77"/>
-    <mergeCell ref="C65:G77"/>
-    <mergeCell ref="H65:J77"/>
-    <mergeCell ref="K65:M77"/>
-    <mergeCell ref="A52:A64"/>
-    <mergeCell ref="B52:B64"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="H27:J39"/>
-    <mergeCell ref="K27:M39"/>
-    <mergeCell ref="C27:G39"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A27:A39"/>
-    <mergeCell ref="B27:B39"/>
-    <mergeCell ref="N14:S14"/>
-    <mergeCell ref="N15:S26"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M26"/>
-    <mergeCell ref="B15:B26"/>
-    <mergeCell ref="C15:G26"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="N65:S77"/>
-    <mergeCell ref="N91:S91"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="H15:J26"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="N93:S93"/>
+    <mergeCell ref="B78:B90"/>
+    <mergeCell ref="C78:G90"/>
+    <mergeCell ref="H78:J90"/>
+    <mergeCell ref="K78:M90"/>
+    <mergeCell ref="N78:S90"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="N92:S92"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:J108"/>
+    <mergeCell ref="K108:M108"/>
+    <mergeCell ref="N108:S108"/>
+    <mergeCell ref="A95:A107"/>
+    <mergeCell ref="B95:B107"/>
+    <mergeCell ref="C95:G107"/>
+    <mergeCell ref="H95:J107"/>
+    <mergeCell ref="K95:M107"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4535,25 +4549,25 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
       <c r="H4" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L4" s="24"/>
       <c r="M4" s="24"/>
@@ -4564,7 +4578,7 @@
       <c r="R4" s="24"/>
       <c r="S4" s="24"/>
       <c r="T4" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4628,30 +4642,30 @@
     </row>
     <row r="7" spans="1:20" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
       <c r="K7" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="N7" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
@@ -4659,19 +4673,11 @@
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
       <c r="T7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="N7:S7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:S6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="K7:M7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="C3:G3"/>
@@ -4681,6 +4687,14 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:S4"/>
     <mergeCell ref="K3:S3"/>
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:S6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="K7:M7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4695,7 +4709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+    <sheetView topLeftCell="C17" workbookViewId="0">
       <selection activeCell="K26" sqref="K26:R26"/>
     </sheetView>
   </sheetViews>
@@ -4710,20 +4724,20 @@
   <sheetData>
     <row r="2" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
@@ -4738,25 +4752,25 @@
       <c r="Q2" s="21"/>
       <c r="R2" s="21"/>
       <c r="S2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
@@ -4771,25 +4785,25 @@
       <c r="Q4" s="21"/>
       <c r="R4" s="21"/>
       <c r="S4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
@@ -4804,18 +4818,18 @@
       <c r="Q6" s="21"/>
       <c r="R6" s="21"/>
       <c r="S6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
@@ -4837,30 +4851,30 @@
       <c r="Q8" s="21"/>
       <c r="R8" s="21"/>
       <c r="S8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
@@ -4870,30 +4884,30 @@
       <c r="Q10" s="21"/>
       <c r="R10" s="21"/>
       <c r="S10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
@@ -4903,18 +4917,18 @@
       <c r="Q12" s="21"/>
       <c r="R12" s="21"/>
       <c r="S12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -4936,30 +4950,30 @@
       <c r="Q14" s="21"/>
       <c r="R14" s="21"/>
       <c r="S14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
       <c r="H16" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
@@ -4969,18 +4983,18 @@
       <c r="Q16" s="21"/>
       <c r="R16" s="21"/>
       <c r="S16" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
@@ -5002,30 +5016,30 @@
       <c r="Q17" s="21"/>
       <c r="R17" s="21"/>
       <c r="S17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I18" s="25"/>
       <c r="J18" s="25"/>
       <c r="K18" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
@@ -5035,30 +5049,30 @@
       <c r="Q18" s="21"/>
       <c r="R18" s="21"/>
       <c r="S18" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
       <c r="H19" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I19" s="25"/>
       <c r="J19" s="25"/>
       <c r="K19" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
@@ -5068,30 +5082,30 @@
       <c r="Q19" s="21"/>
       <c r="R19" s="21"/>
       <c r="S19" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
@@ -5101,30 +5115,30 @@
       <c r="Q20" s="21"/>
       <c r="R20" s="21"/>
       <c r="S20" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
       <c r="H21" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
@@ -5134,30 +5148,30 @@
       <c r="Q21" s="21"/>
       <c r="R21" s="21"/>
       <c r="S21" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
@@ -5167,30 +5181,30 @@
       <c r="Q22" s="21"/>
       <c r="R22" s="21"/>
       <c r="S22" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="22" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
       <c r="K24" s="21" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
@@ -5200,30 +5214,30 @@
       <c r="Q24" s="21"/>
       <c r="R24" s="21"/>
       <c r="S24" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="25" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="21" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
@@ -5233,35 +5247,19 @@
       <c r="Q26" s="21"/>
       <c r="R26" s="21"/>
       <c r="S26" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:R26"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:R18"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:R21"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:J20"/>
@@ -5278,14 +5276,30 @@
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:R16"/>
     <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:R18"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:R22"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:R26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
Correccion de la uri de itinerarios
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="177">
   <si>
     <t>Recurso</t>
   </si>
@@ -531,9 +531,6 @@
     <t>Crea un Itinerario con 3 parametros</t>
   </si>
   <si>
-    <t>itinerario/eliminar/{$clave}</t>
-  </si>
-  <si>
     <t>Encuentra y si existe elimina el itinerario con la clave especificada de lo contrario no se efectua la tarea.</t>
   </si>
   <si>
@@ -968,12 +965,6 @@
 }</t>
   </si>
   <si>
-    <t>http://localhost:8080/cloudBRT/api/admin/itinerario</t>
-  </si>
-  <si>
-    <t>/itinerario</t>
-  </si>
-  <si>
     <t>/buses</t>
   </si>
   <si>
@@ -1137,9 +1128,6 @@
 }</t>
   </si>
   <si>
-    <t>http://localhost:8080/cloudBRT/api/admin/itinerario/I3T3</t>
-  </si>
-  <si>
     <t>{
 "Eliminado":true,
 "RecursoItinerario": "http://localhost:8080/cloudBRT/api/monitoreo/itinerarios"
@@ -1168,6 +1156,15 @@
   "Modificado": true,
   "RecursoConductor": "http://localhost:8080/cloudBRT/api/monitoreo/conductores/1098747294"
 }</t>
+  </si>
+  <si>
+    <t>itinerarios/{$clave}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/admin/itinerarios/I3T3</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/cloudBRT/api/admin/itinerarios</t>
   </si>
 </sst>
 </file>
@@ -1621,8 +1618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F45" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K94" sqref="K94:M94"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,20 +1717,20 @@
     </row>
     <row r="4" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="C4" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
@@ -1753,20 +1750,20 @@
     </row>
     <row r="5" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="20" t="s">
         <v>78</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>79</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
@@ -1786,20 +1783,20 @@
     </row>
     <row r="6" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>87</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
@@ -1819,20 +1816,20 @@
     </row>
     <row r="7" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
@@ -1852,20 +1849,20 @@
     </row>
     <row r="8" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
@@ -1885,20 +1882,20 @@
     </row>
     <row r="9" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
@@ -1918,20 +1915,20 @@
     </row>
     <row r="10" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
@@ -1951,20 +1948,20 @@
     </row>
     <row r="11" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="22" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
@@ -1984,25 +1981,25 @@
     </row>
     <row r="12" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="22" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
@@ -2017,25 +2014,25 @@
     </row>
     <row r="13" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>113</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>114</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="22" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
@@ -2080,25 +2077,25 @@
     </row>
     <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>84</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
       <c r="K15" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
@@ -2358,25 +2355,25 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
       <c r="K27" s="22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
@@ -2658,13 +2655,13 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
@@ -2674,7 +2671,7 @@
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
       <c r="K40" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
@@ -2934,13 +2931,13 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
@@ -2950,7 +2947,7 @@
       <c r="I52" s="21"/>
       <c r="J52" s="21"/>
       <c r="K52" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L52" s="21"/>
       <c r="M52" s="21"/>
@@ -3232,25 +3229,25 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" s="20" t="s">
         <v>115</v>
-      </c>
-      <c r="B65" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C65" s="20" t="s">
-        <v>116</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
       <c r="G65" s="20"/>
       <c r="H65" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I65" s="21"/>
       <c r="J65" s="21"/>
       <c r="K65" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L65" s="21"/>
       <c r="M65" s="21"/>
@@ -3532,25 +3529,25 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D78" s="20"/>
       <c r="E78" s="20"/>
       <c r="F78" s="20"/>
       <c r="G78" s="20"/>
       <c r="H78" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I78" s="21"/>
       <c r="J78" s="21"/>
       <c r="K78" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L78" s="21"/>
       <c r="M78" s="21"/>
@@ -3832,25 +3829,25 @@
     </row>
     <row r="91" spans="1:20" s="5" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
       <c r="F91" s="21"/>
       <c r="G91" s="21"/>
       <c r="H91" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I91" s="21"/>
       <c r="J91" s="21"/>
       <c r="K91" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L91" s="21"/>
       <c r="M91" s="21"/>
@@ -3868,25 +3865,25 @@
     </row>
     <row r="92" spans="1:20" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
       <c r="F92" s="21"/>
       <c r="G92" s="21"/>
       <c r="H92" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I92" s="21"/>
       <c r="J92" s="21"/>
       <c r="K92" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L92" s="21"/>
       <c r="M92" s="21"/>
@@ -3904,25 +3901,25 @@
     </row>
     <row r="93" spans="1:20" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
       <c r="F93" s="21"/>
       <c r="G93" s="21"/>
       <c r="H93" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I93" s="21"/>
       <c r="J93" s="21"/>
       <c r="K93" s="22" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L93" s="21"/>
       <c r="M93" s="21"/>
@@ -3940,25 +3937,25 @@
     </row>
     <row r="94" spans="1:20" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
       <c r="F94" s="21"/>
       <c r="G94" s="21"/>
       <c r="H94" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I94" s="21"/>
       <c r="J94" s="21"/>
       <c r="K94" s="22" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L94" s="21"/>
       <c r="M94" s="21"/>
@@ -3976,25 +3973,25 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>132</v>
+        <v>176</v>
       </c>
       <c r="D95" s="20"/>
       <c r="E95" s="20"/>
       <c r="F95" s="20"/>
       <c r="G95" s="20"/>
       <c r="H95" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I95" s="21"/>
       <c r="J95" s="21"/>
       <c r="K95" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L95" s="21"/>
       <c r="M95" s="21"/>
@@ -4276,13 +4273,13 @@
     </row>
     <row r="108" spans="1:20" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B108" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C108" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="B108" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C108" s="20" t="s">
-        <v>123</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -4292,7 +4289,7 @@
       <c r="I108" s="21"/>
       <c r="J108" s="21"/>
       <c r="K108" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L108" s="21"/>
       <c r="M108" s="21"/>
@@ -4310,6 +4307,89 @@
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:J108"/>
+    <mergeCell ref="K108:M108"/>
+    <mergeCell ref="N108:S108"/>
+    <mergeCell ref="A95:A107"/>
+    <mergeCell ref="B95:B107"/>
+    <mergeCell ref="C95:G107"/>
+    <mergeCell ref="H95:J107"/>
+    <mergeCell ref="K95:M107"/>
+    <mergeCell ref="N93:S93"/>
+    <mergeCell ref="B78:B90"/>
+    <mergeCell ref="C78:G90"/>
+    <mergeCell ref="H78:J90"/>
+    <mergeCell ref="K78:M90"/>
+    <mergeCell ref="N78:S90"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="N92:S92"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="A78:A90"/>
+    <mergeCell ref="K94:M94"/>
+    <mergeCell ref="N94:S94"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="H93:J93"/>
+    <mergeCell ref="K93:M93"/>
+    <mergeCell ref="N95:S107"/>
+    <mergeCell ref="T95:T107"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:R13"/>
+    <mergeCell ref="T65:T77"/>
+    <mergeCell ref="T52:T64"/>
+    <mergeCell ref="N52:S64"/>
+    <mergeCell ref="T78:T90"/>
+    <mergeCell ref="T15:T26"/>
+    <mergeCell ref="N27:S39"/>
+    <mergeCell ref="T27:T39"/>
+    <mergeCell ref="N40:S51"/>
+    <mergeCell ref="T40:T51"/>
+    <mergeCell ref="K40:M51"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="H94:J94"/>
+    <mergeCell ref="A40:A51"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="C40:G51"/>
+    <mergeCell ref="H52:J64"/>
+    <mergeCell ref="K52:M64"/>
+    <mergeCell ref="C52:G64"/>
+    <mergeCell ref="H40:J51"/>
+    <mergeCell ref="A65:A77"/>
+    <mergeCell ref="B65:B77"/>
+    <mergeCell ref="C65:G77"/>
+    <mergeCell ref="H65:J77"/>
+    <mergeCell ref="K65:M77"/>
+    <mergeCell ref="A52:A64"/>
+    <mergeCell ref="B52:B64"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="H27:J39"/>
+    <mergeCell ref="K27:M39"/>
+    <mergeCell ref="C27:G39"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A27:A39"/>
+    <mergeCell ref="B27:B39"/>
+    <mergeCell ref="N14:S14"/>
+    <mergeCell ref="N15:S26"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M26"/>
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="C15:G26"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="A15:A26"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="N65:S77"/>
     <mergeCell ref="N91:S91"/>
@@ -4334,89 +4414,6 @@
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="K12:R12"/>
     <mergeCell ref="H11:J11"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="H27:J39"/>
-    <mergeCell ref="K27:M39"/>
-    <mergeCell ref="C27:G39"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A27:A39"/>
-    <mergeCell ref="B27:B39"/>
-    <mergeCell ref="N14:S14"/>
-    <mergeCell ref="N15:S26"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M26"/>
-    <mergeCell ref="B15:B26"/>
-    <mergeCell ref="C15:G26"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="B40:B51"/>
-    <mergeCell ref="C40:G51"/>
-    <mergeCell ref="H52:J64"/>
-    <mergeCell ref="K52:M64"/>
-    <mergeCell ref="C52:G64"/>
-    <mergeCell ref="H40:J51"/>
-    <mergeCell ref="A65:A77"/>
-    <mergeCell ref="B65:B77"/>
-    <mergeCell ref="C65:G77"/>
-    <mergeCell ref="H65:J77"/>
-    <mergeCell ref="K65:M77"/>
-    <mergeCell ref="A52:A64"/>
-    <mergeCell ref="B52:B64"/>
-    <mergeCell ref="A78:A90"/>
-    <mergeCell ref="K94:M94"/>
-    <mergeCell ref="N94:S94"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="H93:J93"/>
-    <mergeCell ref="K93:M93"/>
-    <mergeCell ref="N95:S107"/>
-    <mergeCell ref="T95:T107"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:R13"/>
-    <mergeCell ref="T65:T77"/>
-    <mergeCell ref="T52:T64"/>
-    <mergeCell ref="N52:S64"/>
-    <mergeCell ref="T78:T90"/>
-    <mergeCell ref="T15:T26"/>
-    <mergeCell ref="N27:S39"/>
-    <mergeCell ref="T27:T39"/>
-    <mergeCell ref="N40:S51"/>
-    <mergeCell ref="T40:T51"/>
-    <mergeCell ref="K40:M51"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="H94:J94"/>
-    <mergeCell ref="A40:A51"/>
-    <mergeCell ref="N93:S93"/>
-    <mergeCell ref="B78:B90"/>
-    <mergeCell ref="C78:G90"/>
-    <mergeCell ref="H78:J90"/>
-    <mergeCell ref="K78:M90"/>
-    <mergeCell ref="N78:S90"/>
-    <mergeCell ref="K91:M91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="N92:S92"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="H91:J91"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:J108"/>
-    <mergeCell ref="K108:M108"/>
-    <mergeCell ref="N108:S108"/>
-    <mergeCell ref="A95:A107"/>
-    <mergeCell ref="B95:B107"/>
-    <mergeCell ref="C95:G107"/>
-    <mergeCell ref="H95:J107"/>
-    <mergeCell ref="K95:M107"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4678,6 +4675,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:S6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="K7:M7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="C3:G3"/>
@@ -4687,14 +4692,6 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:S4"/>
     <mergeCell ref="K3:S3"/>
-    <mergeCell ref="N7:S7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:S6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="K7:M7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4724,13 +4721,13 @@
   <sheetData>
     <row r="2" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
@@ -4757,13 +4754,13 @@
     </row>
     <row r="4" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -4790,13 +4787,13 @@
     </row>
     <row r="6" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -4823,13 +4820,13 @@
     </row>
     <row r="8" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
@@ -4856,13 +4853,13 @@
     </row>
     <row r="10" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -4889,13 +4886,13 @@
     </row>
     <row r="12" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
@@ -4922,13 +4919,13 @@
     </row>
     <row r="14" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -4955,25 +4952,25 @@
     </row>
     <row r="16" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
       <c r="H16" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
@@ -4988,13 +4985,13 @@
     </row>
     <row r="17" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
@@ -5021,25 +5018,25 @@
     </row>
     <row r="18" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I18" s="25"/>
       <c r="J18" s="25"/>
       <c r="K18" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
@@ -5054,25 +5051,25 @@
     </row>
     <row r="19" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
       <c r="H19" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I19" s="25"/>
       <c r="J19" s="25"/>
       <c r="K19" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
@@ -5087,25 +5084,25 @@
     </row>
     <row r="20" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
@@ -5120,25 +5117,25 @@
     </row>
     <row r="21" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
       <c r="H21" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
@@ -5153,25 +5150,25 @@
     </row>
     <row r="22" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
@@ -5186,25 +5183,25 @@
     </row>
     <row r="24" spans="1:19" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="22" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
       <c r="K24" s="21" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
@@ -5219,25 +5216,25 @@
     </row>
     <row r="26" spans="1:19" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="25" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
@@ -5252,14 +5249,30 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:R18"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:R22"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:R26"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:J20"/>
@@ -5276,30 +5289,14 @@
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:R16"/>
     <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:R26"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:R18"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:R21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
Se corrigio un bug que impedia la eliminacion correcta de un itinerario
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="178">
   <si>
     <t>Recurso</t>
   </si>
@@ -951,12 +951,6 @@
   </si>
   <si>
     <t>{
-  "Encontrado": true,
-  "RecursoItinerarios": "http://localhost:8080/cloudBRT/api/monitoreo/itinerarios/IT-3"
-}</t>
-  </si>
-  <si>
-    <t>{
 "Clave":"IT-3",
 "Conductor":"1098747294",
 "Placa":"AMB123",
@@ -1165,6 +1159,18 @@
   </si>
   <si>
     <t>http://localhost:8080/cloudBRT/api/admin/itinerarios</t>
+  </si>
+  <si>
+    <t>{
+  "Creado": true,
+  "RecursoItinerarios": "http://localhost:8080/cloudBRT/api/monitoreo/itinerarios/IT-3"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "Eliminado": true,
+  "RecursoConductor": "http://localhost:8080/cloudBRT/api/monitoreo/conductores/1098747294"
+}</t>
   </si>
 </sst>
 </file>
@@ -1618,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:J4"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,7 +1736,7 @@
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
@@ -1763,7 +1769,7 @@
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
@@ -1829,7 +1835,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
@@ -1862,7 +1868,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
@@ -1895,7 +1901,7 @@
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
@@ -1961,7 +1967,7 @@
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
@@ -1981,20 +1987,20 @@
     </row>
     <row r="12" spans="1:20" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
@@ -2027,7 +2033,7 @@
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
@@ -2095,7 +2101,7 @@
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
       <c r="K15" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
@@ -2373,7 +2379,7 @@
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
       <c r="K27" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
@@ -3919,7 +3925,7 @@
       <c r="I93" s="21"/>
       <c r="J93" s="21"/>
       <c r="K93" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L93" s="21"/>
       <c r="M93" s="21"/>
@@ -3955,7 +3961,7 @@
       <c r="I94" s="21"/>
       <c r="J94" s="21"/>
       <c r="K94" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L94" s="21"/>
       <c r="M94" s="21"/>
@@ -3973,25 +3979,25 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B95" s="21" t="s">
         <v>84</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D95" s="20"/>
       <c r="E95" s="20"/>
       <c r="F95" s="20"/>
       <c r="G95" s="20"/>
       <c r="H95" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I95" s="21"/>
       <c r="J95" s="21"/>
       <c r="K95" s="22" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="L95" s="21"/>
       <c r="M95" s="21"/>
@@ -4289,7 +4295,7 @@
       <c r="I108" s="21"/>
       <c r="J108" s="21"/>
       <c r="K108" s="22" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="L108" s="21"/>
       <c r="M108" s="21"/>
@@ -4307,28 +4313,67 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:J108"/>
-    <mergeCell ref="K108:M108"/>
-    <mergeCell ref="N108:S108"/>
-    <mergeCell ref="A95:A107"/>
-    <mergeCell ref="B95:B107"/>
-    <mergeCell ref="C95:G107"/>
-    <mergeCell ref="H95:J107"/>
-    <mergeCell ref="K95:M107"/>
-    <mergeCell ref="N93:S93"/>
-    <mergeCell ref="B78:B90"/>
-    <mergeCell ref="C78:G90"/>
-    <mergeCell ref="H78:J90"/>
-    <mergeCell ref="K78:M90"/>
-    <mergeCell ref="N78:S90"/>
-    <mergeCell ref="K91:M91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="N92:S92"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="N65:S77"/>
+    <mergeCell ref="N91:S91"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="H15:J26"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="H27:J39"/>
+    <mergeCell ref="K27:M39"/>
+    <mergeCell ref="C27:G39"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A27:A39"/>
+    <mergeCell ref="B27:B39"/>
+    <mergeCell ref="N14:S14"/>
+    <mergeCell ref="N15:S26"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M26"/>
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="C15:G26"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="C40:G51"/>
+    <mergeCell ref="H52:J64"/>
+    <mergeCell ref="K52:M64"/>
+    <mergeCell ref="C52:G64"/>
+    <mergeCell ref="H40:J51"/>
+    <mergeCell ref="A65:A77"/>
+    <mergeCell ref="B65:B77"/>
+    <mergeCell ref="C65:G77"/>
+    <mergeCell ref="H65:J77"/>
+    <mergeCell ref="K65:M77"/>
+    <mergeCell ref="A52:A64"/>
+    <mergeCell ref="B52:B64"/>
     <mergeCell ref="A78:A90"/>
     <mergeCell ref="K94:M94"/>
     <mergeCell ref="N94:S94"/>
@@ -4353,67 +4398,28 @@
     <mergeCell ref="C94:G94"/>
     <mergeCell ref="H94:J94"/>
     <mergeCell ref="A40:A51"/>
-    <mergeCell ref="B40:B51"/>
-    <mergeCell ref="C40:G51"/>
-    <mergeCell ref="H52:J64"/>
-    <mergeCell ref="K52:M64"/>
-    <mergeCell ref="C52:G64"/>
-    <mergeCell ref="H40:J51"/>
-    <mergeCell ref="A65:A77"/>
-    <mergeCell ref="B65:B77"/>
-    <mergeCell ref="C65:G77"/>
-    <mergeCell ref="H65:J77"/>
-    <mergeCell ref="K65:M77"/>
-    <mergeCell ref="A52:A64"/>
-    <mergeCell ref="B52:B64"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="H27:J39"/>
-    <mergeCell ref="K27:M39"/>
-    <mergeCell ref="C27:G39"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A27:A39"/>
-    <mergeCell ref="B27:B39"/>
-    <mergeCell ref="N14:S14"/>
-    <mergeCell ref="N15:S26"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M26"/>
-    <mergeCell ref="B15:B26"/>
-    <mergeCell ref="C15:G26"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="N65:S77"/>
-    <mergeCell ref="N91:S91"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="H15:J26"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="N93:S93"/>
+    <mergeCell ref="B78:B90"/>
+    <mergeCell ref="C78:G90"/>
+    <mergeCell ref="H78:J90"/>
+    <mergeCell ref="K78:M90"/>
+    <mergeCell ref="N78:S90"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="N92:S92"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:J108"/>
+    <mergeCell ref="K108:M108"/>
+    <mergeCell ref="N108:S108"/>
+    <mergeCell ref="A95:A107"/>
+    <mergeCell ref="B95:B107"/>
+    <mergeCell ref="C95:G107"/>
+    <mergeCell ref="H95:J107"/>
+    <mergeCell ref="K95:M107"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4675,14 +4681,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="N7:S7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:S6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="K7:M7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="C3:G3"/>
@@ -4692,6 +4690,14 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:S4"/>
     <mergeCell ref="K3:S3"/>
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:S6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="K7:M7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4721,13 +4727,13 @@
   <sheetData>
     <row r="2" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
@@ -4760,7 +4766,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -4787,13 +4793,13 @@
     </row>
     <row r="6" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -4820,13 +4826,13 @@
     </row>
     <row r="8" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
@@ -4859,7 +4865,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -4886,13 +4892,13 @@
     </row>
     <row r="12" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
@@ -4925,7 +4931,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -4952,13 +4958,13 @@
     </row>
     <row r="16" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
@@ -4985,13 +4991,13 @@
     </row>
     <row r="17" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
@@ -5018,13 +5024,13 @@
     </row>
     <row r="18" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
@@ -5051,13 +5057,13 @@
     </row>
     <row r="19" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -5084,13 +5090,13 @@
     </row>
     <row r="20" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -5117,13 +5123,13 @@
     </row>
     <row r="21" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -5150,13 +5156,13 @@
     </row>
     <row r="22" spans="1:19" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -5189,19 +5195,19 @@
         <v>3</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
       <c r="K24" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
@@ -5222,19 +5228,19 @@
         <v>3</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
@@ -5249,30 +5255,14 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:R26"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:R18"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:R21"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:J20"/>
@@ -5289,14 +5279,30 @@
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:R16"/>
     <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:R18"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:R22"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:R26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
Se elimino la db debido al tamaño y se renombro la variable que cuenta las peticiones
</commit_message>
<xml_diff>
--- a/documentacion.xlsx
+++ b/documentacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15195" windowHeight="4170" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15195" windowHeight="4170"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="1" r:id="rId1"/>
@@ -1647,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T110"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4370,31 +4370,67 @@
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="H110:J110"/>
-    <mergeCell ref="K110:S110"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="H108:J108"/>
-    <mergeCell ref="K108:M108"/>
-    <mergeCell ref="N108:S108"/>
-    <mergeCell ref="A95:A107"/>
-    <mergeCell ref="B95:B107"/>
-    <mergeCell ref="C95:G107"/>
-    <mergeCell ref="H95:J107"/>
-    <mergeCell ref="K95:M107"/>
-    <mergeCell ref="N93:S93"/>
-    <mergeCell ref="B78:B90"/>
-    <mergeCell ref="C78:G90"/>
-    <mergeCell ref="H78:J90"/>
-    <mergeCell ref="K78:M90"/>
-    <mergeCell ref="N78:S90"/>
-    <mergeCell ref="K91:M91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="N92:S92"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="N65:S77"/>
+    <mergeCell ref="N91:S91"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="H15:J26"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="H27:J39"/>
+    <mergeCell ref="K27:M39"/>
+    <mergeCell ref="C27:G39"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A27:A39"/>
+    <mergeCell ref="B27:B39"/>
+    <mergeCell ref="N14:S14"/>
+    <mergeCell ref="N15:S26"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M26"/>
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="C15:G26"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="C40:G51"/>
+    <mergeCell ref="H52:J64"/>
+    <mergeCell ref="K52:M64"/>
+    <mergeCell ref="C52:G64"/>
+    <mergeCell ref="H40:J51"/>
+    <mergeCell ref="A65:A77"/>
+    <mergeCell ref="B65:B77"/>
+    <mergeCell ref="C65:G77"/>
+    <mergeCell ref="H65:J77"/>
+    <mergeCell ref="K65:M77"/>
+    <mergeCell ref="A52:A64"/>
+    <mergeCell ref="B52:B64"/>
     <mergeCell ref="A78:A90"/>
     <mergeCell ref="K94:M94"/>
     <mergeCell ref="N94:S94"/>
@@ -4419,67 +4455,31 @@
     <mergeCell ref="C94:G94"/>
     <mergeCell ref="H94:J94"/>
     <mergeCell ref="A40:A51"/>
-    <mergeCell ref="B40:B51"/>
-    <mergeCell ref="C40:G51"/>
-    <mergeCell ref="H52:J64"/>
-    <mergeCell ref="K52:M64"/>
-    <mergeCell ref="C52:G64"/>
-    <mergeCell ref="H40:J51"/>
-    <mergeCell ref="A65:A77"/>
-    <mergeCell ref="B65:B77"/>
-    <mergeCell ref="C65:G77"/>
-    <mergeCell ref="H65:J77"/>
-    <mergeCell ref="K65:M77"/>
-    <mergeCell ref="A52:A64"/>
-    <mergeCell ref="B52:B64"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="H27:J39"/>
-    <mergeCell ref="K27:M39"/>
-    <mergeCell ref="C27:G39"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A27:A39"/>
-    <mergeCell ref="B27:B39"/>
-    <mergeCell ref="N14:S14"/>
-    <mergeCell ref="N15:S26"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M26"/>
-    <mergeCell ref="B15:B26"/>
-    <mergeCell ref="C15:G26"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="N65:S77"/>
-    <mergeCell ref="N91:S91"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="H15:J26"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="N93:S93"/>
+    <mergeCell ref="B78:B90"/>
+    <mergeCell ref="C78:G90"/>
+    <mergeCell ref="H78:J90"/>
+    <mergeCell ref="K78:M90"/>
+    <mergeCell ref="N78:S90"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="N92:S92"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:J110"/>
+    <mergeCell ref="K110:S110"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:J108"/>
+    <mergeCell ref="K108:M108"/>
+    <mergeCell ref="N108:S108"/>
+    <mergeCell ref="A95:A107"/>
+    <mergeCell ref="B95:B107"/>
+    <mergeCell ref="C95:G107"/>
+    <mergeCell ref="H95:J107"/>
+    <mergeCell ref="K95:M107"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4516,7 +4516,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:G7"/>
+      <selection activeCell="H7" sqref="H7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4710,6 +4710,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="A5:R5"/>
+    <mergeCell ref="K3:S3"/>
     <mergeCell ref="N7:S7"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:J7"/>
@@ -4718,12 +4724,6 @@
     <mergeCell ref="N6:S6"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="K7:M7"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="A5:R5"/>
-    <mergeCell ref="K3:S3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -4738,7 +4738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="H22" sqref="H22:J22"/>
     </sheetView>
   </sheetViews>
@@ -5281,30 +5281,14 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:R26"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:R18"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:R21"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:J20"/>
@@ -5321,14 +5305,30 @@
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:R16"/>
     <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:R18"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:R22"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:R8"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:R26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -5358,7 +5358,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:R5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5556,13 +5556,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:S4"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:S6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="K7:M7"/>
@@ -5573,6 +5566,13 @@
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:S3"/>
     <mergeCell ref="A5:R5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:S4"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:S6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>

</xml_diff>